<commit_message>
reports cases added in sogo
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DAFBEF-9F79-404C-ADB0-F2BFFCF5B401}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11040" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -12,17 +13,26 @@
     <sheet name="Users" sheetId="2" r:id="rId3"/>
     <sheet name="SmokeTC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="203">
   <si>
     <t>Environment</t>
   </si>
@@ -486,9 +496,6 @@
     <t>emailtemplatere</t>
   </si>
   <si>
-    <t>Sanity_TC3</t>
-  </si>
-  <si>
     <t>DMX</t>
   </si>
   <si>
@@ -504,33 +511,21 @@
     <t>Reminder_EXE DP RA</t>
   </si>
   <si>
-    <t>Sanity_TC4</t>
-  </si>
-  <si>
     <t>To send Platfrom Invite &amp; PF reminder</t>
   </si>
   <si>
-    <t>Sanity_TC5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Send SMS invites and reminder </t>
   </si>
   <si>
     <t>SMS numbers.xlsx</t>
   </si>
   <si>
-    <t>Sanity_TC6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Downloading SAP </t>
   </si>
   <si>
     <t>survey should be downloaded</t>
   </si>
   <si>
-    <t>Sanity_TC7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Create new list </t>
   </si>
   <si>
@@ -576,9 +571,6 @@
     <t>DMx PF DP</t>
   </si>
   <si>
-    <t>Sanity_TC8</t>
-  </si>
-  <si>
     <t>Test Invite</t>
   </si>
   <si>
@@ -588,9 +580,6 @@
     <t>Copy (4) of switch of DP survey from 26th October</t>
   </si>
   <si>
-    <t>Sanity_TC9</t>
-  </si>
-  <si>
     <t>DAR</t>
   </si>
   <si>
@@ -609,14 +598,56 @@
     <t>welcome29</t>
   </si>
   <si>
-    <t>Sanity_TC10</t>
+    <t>Smoke_TC3</t>
+  </si>
+  <si>
+    <t>Smoke_TC4</t>
+  </si>
+  <si>
+    <t>Smoke_TC5</t>
+  </si>
+  <si>
+    <t>Smoke_TC6</t>
+  </si>
+  <si>
+    <t>Smoke_TC7</t>
+  </si>
+  <si>
+    <t>Smoke_TC8</t>
+  </si>
+  <si>
+    <t>Smoke_TC9</t>
+  </si>
+  <si>
+    <t>Smoke_TC10</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>OOPS! Something went wrong! Page displayed on sending the reminder</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dp test invites [18 records] list not present </t>
+  </si>
+  <si>
+    <t>DP PF list [5 records] list not present</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>Reminder email template not provided</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,8 +680,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -676,6 +713,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,7 +796,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -767,6 +816,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1040,14 +1092,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1055,13 +1107,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1089,21 +1141,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1131,15 +1183,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1147,7 +1199,7 @@
     <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1175,32 +1227,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1209,15 +1261,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CP11"/>
+  <dimension ref="A1:CO11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1237,11 +1289,10 @@
     <col min="16" max="16" width="15" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="86" max="86" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94">
+    <row r="1" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1498,31 +1549,28 @@
         <v>146</v>
       </c>
       <c r="CH1" s="9" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="CI1" s="9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="CJ1" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="CK1" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="CL1" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="CM1" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="CN1" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="CO1" s="9" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:94">
+    <row r="2" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1545,7 +1593,9 @@
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="13"/>
+      <c r="I2" s="21" t="s">
+        <v>201</v>
+      </c>
       <c r="J2" s="13"/>
       <c r="K2" s="1" t="s">
         <v>28</v>
@@ -1631,9 +1681,8 @@
       <c r="CL2" s="6"/>
       <c r="CM2" s="6"/>
       <c r="CN2" s="6"/>
-      <c r="CO2" s="6"/>
     </row>
-    <row r="3" spans="1:94">
+    <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -1656,7 +1705,9 @@
       <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="19" t="s">
+        <v>196</v>
+      </c>
       <c r="J3" s="13"/>
       <c r="K3" s="1"/>
       <c r="L3" s="4"/>
@@ -1820,11 +1871,10 @@
       <c r="CL3" s="6"/>
       <c r="CM3" s="6"/>
       <c r="CN3" s="6"/>
-      <c r="CO3" s="6"/>
     </row>
-    <row r="4" spans="1:94">
+    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -1836,17 +1886,21 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
+        <v>156</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>202</v>
+      </c>
       <c r="K4" s="1"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1922,32 +1976,31 @@
       <c r="CE4" s="11"/>
       <c r="CF4" s="11"/>
       <c r="CG4" s="11"/>
-      <c r="CH4" s="11"/>
-      <c r="CI4" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="CJ4" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="CK4" s="15" t="s">
-        <v>176</v>
+      <c r="CH4" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="CI4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="CJ4" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="CK4" s="12" t="s">
+        <v>172</v>
       </c>
       <c r="CL4" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="CM4" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="CN4" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="CN4" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="CO4" s="16" t="s">
-        <v>159</v>
-      </c>
     </row>
-    <row r="5" spans="1:94">
+    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>160</v>
+        <v>189</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -1959,17 +2012,21 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+        <v>156</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>200</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
@@ -2045,32 +2102,31 @@
       <c r="CE5" s="11"/>
       <c r="CF5" s="11"/>
       <c r="CG5" s="11"/>
-      <c r="CH5" s="11"/>
+      <c r="CH5" s="12" t="s">
+        <v>174</v>
+      </c>
       <c r="CI5" s="12" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="CJ5" s="12" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="CK5" s="12" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="CL5" s="12" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="CM5" s="12" t="s">
-        <v>17</v>
+        <v>177</v>
       </c>
       <c r="CN5" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="CO5" s="12" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:94">
+    <row r="6" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -2082,17 +2138,21 @@
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+        <v>156</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>197</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -2168,22 +2228,21 @@
       <c r="CE6" s="11"/>
       <c r="CF6" s="11"/>
       <c r="CG6" s="11"/>
-      <c r="CH6" s="11"/>
-      <c r="CI6" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="CJ6" s="12"/>
-      <c r="CK6" s="12" t="s">
-        <v>164</v>
-      </c>
+      <c r="CH6" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="CI6" s="12"/>
+      <c r="CJ6" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="CK6" s="12"/>
       <c r="CL6" s="12"/>
       <c r="CM6" s="12"/>
       <c r="CN6" s="12"/>
-      <c r="CO6" s="12"/>
     </row>
-    <row r="7" spans="1:94">
+    <row r="7" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -2195,17 +2254,21 @@
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
+        <v>163</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>200</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -2281,24 +2344,23 @@
       <c r="CE7" s="11"/>
       <c r="CF7" s="11"/>
       <c r="CG7" s="11"/>
-      <c r="CH7" s="11"/>
-      <c r="CI7" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="CJ7" s="12"/>
-      <c r="CK7" s="12" t="s">
-        <v>181</v>
-      </c>
+      <c r="CH7" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="CI7" s="12"/>
+      <c r="CJ7" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="CK7" s="12"/>
       <c r="CL7" s="12"/>
-      <c r="CM7" s="12"/>
-      <c r="CN7" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="CO7" s="12"/>
+      <c r="CM7" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="CN7" s="12"/>
     </row>
-    <row r="8" spans="1:94">
+    <row r="8" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
@@ -2310,16 +2372,18 @@
         <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I8" s="13"/>
+        <v>163</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>196</v>
+      </c>
       <c r="J8" s="13"/>
       <c r="K8" s="1"/>
       <c r="L8" s="10"/>
@@ -2396,24 +2460,23 @@
       <c r="CE8" s="11"/>
       <c r="CF8" s="11"/>
       <c r="CG8" s="11"/>
-      <c r="CH8" s="11"/>
-      <c r="CI8" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="CJ8" s="12"/>
-      <c r="CK8" s="12" t="s">
-        <v>170</v>
-      </c>
+      <c r="CH8" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="CI8" s="12"/>
+      <c r="CJ8" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="CK8" s="12"/>
       <c r="CL8" s="12"/>
-      <c r="CM8" s="12"/>
-      <c r="CN8" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="CO8" s="12"/>
+      <c r="CM8" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="CN8" s="12"/>
     </row>
-    <row r="9" spans="1:94">
+    <row r="9" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>3</v>
@@ -2425,17 +2488,21 @@
         <v>17</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="1"/>
+        <v>156</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>199</v>
+      </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -2471,7 +2538,9 @@
       <c r="AQ9" s="1"/>
       <c r="AR9" s="1"/>
       <c r="AS9" s="1"/>
-      <c r="AT9" s="1"/>
+      <c r="AT9" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="AU9" s="1"/>
       <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
@@ -2511,34 +2580,31 @@
       <c r="CE9" s="1"/>
       <c r="CF9" s="1"/>
       <c r="CG9" s="1"/>
-      <c r="CH9" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="CI9" s="1">
+      <c r="CH9" s="1">
         <v>313</v>
       </c>
-      <c r="CJ9" s="12" t="s">
+      <c r="CI9" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="CJ9" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="CK9" s="11" t="s">
-        <v>186</v>
+      <c r="CK9" s="12" t="s">
+        <v>177</v>
       </c>
       <c r="CL9" s="12" t="s">
-        <v>182</v>
+        <v>17</v>
       </c>
       <c r="CM9" s="12" t="s">
-        <v>17</v>
+        <v>177</v>
       </c>
       <c r="CN9" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="CO9" s="12" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:94">
-      <c r="A10" s="11" t="s">
-        <v>188</v>
+    <row r="10" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>3</v>
@@ -2553,11 +2619,13 @@
         <v>7</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="I10" s="21" t="s">
+        <v>201</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -2595,10 +2663,10 @@
       <c r="AR10" s="1"/>
       <c r="AS10" s="1"/>
       <c r="AT10" s="17" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="AV10" s="1"/>
       <c r="AW10" s="1"/>
@@ -2646,17 +2714,16 @@
       <c r="CK10" s="1"/>
       <c r="CL10" s="1"/>
       <c r="CM10" s="1"/>
-      <c r="CN10" s="1"/>
-      <c r="CO10" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="CP10" s="18">
+      <c r="CN10" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="CO10" s="18">
         <f>DATE(2021,1,28)</f>
         <v>44224</v>
       </c>
     </row>
-    <row r="11" spans="1:94">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>195</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -2672,11 +2739,13 @@
         <v>7</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="I11" s="21" t="s">
+        <v>201</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -2714,10 +2783,10 @@
       <c r="AR11" s="1"/>
       <c r="AS11" s="1"/>
       <c r="AT11" s="17" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="AU11" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="AV11" s="1"/>
       <c r="AW11" s="1"/>
@@ -2765,14 +2834,14 @@
       <c r="CK11" s="1"/>
       <c r="CL11" s="1"/>
       <c r="CM11" s="1"/>
-      <c r="CN11" s="1"/>
-      <c r="CO11" s="1" t="s">
-        <v>192</v>
+      <c r="CN11" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com"/>
+    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
all reports cases added in all suites except DAR
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DAFBEF-9F79-404C-ADB0-F2BFFCF5B401}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00299EBE-191D-41C7-A291-6C58923F2F45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="240">
   <si>
     <t>Environment</t>
   </si>
@@ -641,13 +641,174 @@
   </si>
   <si>
     <t>Reminder email template not provided</t>
+  </si>
+  <si>
+    <t>RMX</t>
+  </si>
+  <si>
+    <t>Omni report</t>
+  </si>
+  <si>
+    <t>1. Click on Slideshow icon, it will open in new i-Frame. Click on Email, enter given email id in To field and then send the email.
+2. Click on Save button and save the report named as OMNI DP Today's Date
+3. Click on Add report to canvas
+4. Export omni report
+"5. Click on email report. Enter report title as 'OMNI DP Today's date'.
+Enter given email ID in To field, click on continue and sent the email report."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OMNI DP  - </t>
+  </si>
+  <si>
+    <t>jreddy@zarca.com</t>
+  </si>
+  <si>
+    <t>Advance frequency report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1. Click on Frequency button and select 'Advance Frequency' report in drop down
+2. Select All Questions on Survey Questions page and click on Continue.
+3. Reorder the questions on Reorder Question page and then click on Continue.
+4. Check Display reports with data tables, Display Question Numbers, Display Weighted Score/Average for Rating Questions on Properties page and then click on Continue
+5. Click on Generate button on Data Sources and Filters page.
+6. Click on Slideshow icon, it will open in new i-Frame. Click on Email, enter given email id in To field and then send the email.
+7. Click on Save button and save the report named as 'Advance Freq DP Today's Date'
+8. Click on Download button to export the report.
+"9. Click on email report. Enter report title as 'Adv freq DP Today's date'.
+Enter given email ID in To field, click on continue and sent the email report."
+</t>
+  </si>
+  <si>
+    <t>Advance Freq DP</t>
+  </si>
+  <si>
+    <t>Smoke_TC11</t>
+  </si>
+  <si>
+    <t>Individual report</t>
+  </si>
+  <si>
+    <t>1. Click on Raw Data button and select 'Individual' report in drop down
+2. Select All Questions on Survey Questions page and click on Continue.
+3. Click on Continue button on Select Report Properties page.
+4. Click on Generate on Select Filter page.
+5. Click on Download button to export the report.
+6. Click on Save button and save the report named as 'Individual DP Today's Date'
+"7. Click on email report. Enter report title as 'Individual DP Today's date'.
+Enter given email ID in To field, click on continue and sent the email report."</t>
+  </si>
+  <si>
+    <t>Individual DP</t>
+  </si>
+  <si>
+    <t>Smoke_TC12</t>
+  </si>
+  <si>
+    <t>Response table report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on Raw Data button and select 'Response table' report in drop down
+2. Select All Questions on Survey Questions page and click on Continue.
+3. Click on Continue button on Select Report Properties page.
+4. Click on Generate on Select Filter page.
+5. Click on Download button to export the report.
+6. Click on Save button and save the report named as 'Response table DP Today's Date'
+"7. Click on email report. Enter report title as 'Response table DP Today's date'.
+Enter given email ID in To field, click on continue and sent the email report."
+</t>
+  </si>
+  <si>
+    <t>Response table DP</t>
+  </si>
+  <si>
+    <t>Smoke_TC13</t>
+  </si>
+  <si>
+    <t>Segmentation report</t>
+  </si>
+  <si>
+    <t>1. Click on Segementation button.
+2. Select Q.1 as segment question. Once the question is selected, select all answer options in same question. Click on Continue
+3. Select All Questions on Survey Questions page and click on Continue.
+4. Check Display reports with data tables, Display Question Numbers, Display Weighted Score/Average for Rating Questions on Properties page and then click on Continue
+5. Click on Continue on 'Comparison Segment Data'
+6. Click on Continue on Customize Cover Page.
+7. Enter the given email id in To field, check All segment reports as multiple Word documents in a zipped file, Individual segment report in separate Word document anf then click on Generate.</t>
+  </si>
+  <si>
+    <t>Smoke_TC14</t>
+  </si>
+  <si>
+    <t>Engagement report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on Special Reports button and select 'Engagement' report in drop down
+"2. Enter Engagement report DP Today's date as input text in Who are the participants in this study? field. 
+"
+3. Set Nmax as 10,000 and click on Continue.
+4. Select Q.16, 17, 18 as Engagement question (including sub questions) and Click on Continue.
+5. Select Q.19 as Driver question and Click on Continue.
+6. Toggle on Do you want to include additional questions? and Select Q.1 as Additional question and then click on Continue.
+7. Toggle on Individual Composition Report and Select Q.2 as Composion question and then click on Continue.
+8. Toggle on Do you want to generate group-specific reports? and Select Q.2 and name as Location .
+9, Click on Add More, and Select Q.4 and name as School and then click on Continue.
+10. Click on Generate and select export format 
+11. Enter the given email id in pop up and then click on Submit.
+12, Accept the alert.
+</t>
+  </si>
+  <si>
+    <t>Engagement report DP</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Smoke_TC15</t>
+  </si>
+  <si>
+    <t>Smoke_TC16</t>
+  </si>
+  <si>
+    <t>surveyTitle</t>
+  </si>
+  <si>
+    <t>All Question survey</t>
+  </si>
+  <si>
+    <t>Q6. DD: What's your household income?</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Q 3</t>
+  </si>
+  <si>
+    <t>Q 2,Q 4,Q 5</t>
+  </si>
+  <si>
+    <t>Q 2</t>
+  </si>
+  <si>
+    <t>Need discussion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,6 +843,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -792,11 +960,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -815,14 +986,20 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{E0C9F20A-3C63-41E3-B488-667155B99753}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{BEFE91A1-6694-4EFC-B4C7-79AC9427A142}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{E3D7501D-72D4-41B1-89B8-6CC3B051C17C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1188,7 +1365,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1242,8 +1419,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
+      <c r="A4" s="24" t="s">
+        <v>203</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>186</v>
@@ -1252,21 +1429,22 @@
         <v>187</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CO11"/>
+  <dimension ref="A1:CO17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1467,7 @@
     <col min="16" max="16" width="15" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="92" max="93" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:93" x14ac:dyDescent="0.25">
@@ -1569,6 +1747,9 @@
       <c r="CN1" s="9" t="s">
         <v>153</v>
       </c>
+      <c r="CO1" s="9" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="2" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1593,7 +1774,7 @@
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>201</v>
       </c>
       <c r="J2" s="13"/>
@@ -1681,6 +1862,7 @@
       <c r="CL2" s="6"/>
       <c r="CM2" s="6"/>
       <c r="CN2" s="6"/>
+      <c r="CO2" s="6"/>
     </row>
     <row r="3" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1705,7 +1887,7 @@
       <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="18" t="s">
         <v>196</v>
       </c>
       <c r="J3" s="13"/>
@@ -1871,6 +2053,7 @@
       <c r="CL3" s="6"/>
       <c r="CM3" s="6"/>
       <c r="CN3" s="6"/>
+      <c r="CO3" s="6"/>
     </row>
     <row r="4" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1895,7 +2078,7 @@
       <c r="H4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="19" t="s">
         <v>198</v>
       </c>
       <c r="J4" s="13" t="s">
@@ -1997,6 +2180,7 @@
       <c r="CN4" s="16" t="s">
         <v>158</v>
       </c>
+      <c r="CO4" s="16"/>
     </row>
     <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2021,7 +2205,7 @@
       <c r="H5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="19" t="s">
         <v>198</v>
       </c>
       <c r="J5" s="12" t="s">
@@ -2123,6 +2307,7 @@
       <c r="CN5" s="12" t="s">
         <v>178</v>
       </c>
+      <c r="CO5" s="12"/>
     </row>
     <row r="6" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2147,7 +2332,7 @@
       <c r="H6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>198</v>
       </c>
       <c r="J6" s="13" t="s">
@@ -2239,6 +2424,7 @@
       <c r="CL6" s="12"/>
       <c r="CM6" s="12"/>
       <c r="CN6" s="12"/>
+      <c r="CO6" s="12"/>
     </row>
     <row r="7" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2263,7 +2449,7 @@
       <c r="H7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I7" s="20" t="s">
+      <c r="I7" s="19" t="s">
         <v>198</v>
       </c>
       <c r="J7" s="12" t="s">
@@ -2357,6 +2543,7 @@
         <v>157</v>
       </c>
       <c r="CN7" s="12"/>
+      <c r="CO7" s="12"/>
     </row>
     <row r="8" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -2381,7 +2568,7 @@
       <c r="H8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="18" t="s">
         <v>196</v>
       </c>
       <c r="J8" s="13"/>
@@ -2473,6 +2660,7 @@
         <v>166</v>
       </c>
       <c r="CN8" s="12"/>
+      <c r="CO8" s="12"/>
     </row>
     <row r="9" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2497,7 +2685,7 @@
       <c r="H9" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="19" t="s">
         <v>198</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -2601,242 +2789,978 @@
       <c r="CN9" s="12" t="s">
         <v>178</v>
       </c>
+      <c r="CO9" s="12"/>
     </row>
     <row r="10" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
-      <c r="AM10" s="1"/>
-      <c r="AN10" s="1"/>
-      <c r="AO10" s="1"/>
-      <c r="AP10" s="1"/>
-      <c r="AQ10" s="1"/>
-      <c r="AR10" s="1"/>
-      <c r="AS10" s="1"/>
-      <c r="AT10" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="AU10" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AV10" s="1"/>
-      <c r="AW10" s="1"/>
-      <c r="AX10" s="1"/>
-      <c r="AY10" s="1"/>
-      <c r="AZ10" s="1"/>
-      <c r="BA10" s="1"/>
-      <c r="BB10" s="1"/>
-      <c r="BC10" s="1"/>
-      <c r="BD10" s="1"/>
-      <c r="BE10" s="1"/>
-      <c r="BF10" s="1"/>
-      <c r="BG10" s="1"/>
-      <c r="BH10" s="1"/>
-      <c r="BI10" s="1"/>
-      <c r="BJ10" s="1"/>
-      <c r="BK10" s="1"/>
-      <c r="BL10" s="1"/>
-      <c r="BM10" s="1"/>
-      <c r="BN10" s="1"/>
-      <c r="BO10" s="1"/>
-      <c r="BP10" s="1"/>
-      <c r="BQ10" s="1"/>
-      <c r="BR10" s="1"/>
-      <c r="BS10" s="1"/>
-      <c r="BT10" s="1"/>
-      <c r="BU10" s="1"/>
-      <c r="BV10" s="1"/>
-      <c r="BW10" s="1"/>
-      <c r="BX10" s="1"/>
-      <c r="BY10" s="1"/>
-      <c r="BZ10" s="1"/>
-      <c r="CA10" s="1"/>
-      <c r="CB10" s="1"/>
-      <c r="CC10" s="1"/>
-      <c r="CD10" s="1"/>
-      <c r="CE10" s="1"/>
-      <c r="CF10" s="1"/>
-      <c r="CG10" s="1"/>
-      <c r="CH10" s="11">
-        <v>91</v>
-      </c>
-      <c r="CI10" s="1"/>
-      <c r="CJ10" s="1"/>
-      <c r="CK10" s="1"/>
-      <c r="CL10" s="1"/>
-      <c r="CM10" s="1"/>
-      <c r="CN10" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="CO10" s="18">
-        <f>DATE(2021,1,28)</f>
-        <v>44224</v>
+      <c r="E10" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="H10" s="21"/>
+      <c r="I10" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="J10" s="22"/>
+      <c r="K10" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="23"/>
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="23"/>
+      <c r="AB10" s="23"/>
+      <c r="AC10" s="23"/>
+      <c r="AD10" s="23"/>
+      <c r="AE10" s="23"/>
+      <c r="AF10" s="23"/>
+      <c r="AG10" s="23"/>
+      <c r="AH10" s="23"/>
+      <c r="AI10" s="23"/>
+      <c r="AJ10" s="23"/>
+      <c r="AK10" s="23"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="21"/>
+      <c r="AO10" s="21"/>
+      <c r="AP10" s="21"/>
+      <c r="AQ10" s="21"/>
+      <c r="AR10" s="21"/>
+      <c r="AS10" s="21"/>
+      <c r="AT10" s="21"/>
+      <c r="AU10" s="21"/>
+      <c r="AV10" s="21"/>
+      <c r="AW10" s="21"/>
+      <c r="AX10" s="21"/>
+      <c r="AY10" s="21"/>
+      <c r="AZ10" s="21"/>
+      <c r="BA10" s="21"/>
+      <c r="BB10" s="21"/>
+      <c r="BC10" s="21"/>
+      <c r="BD10" s="21"/>
+      <c r="BE10" s="23"/>
+      <c r="BF10" s="21"/>
+      <c r="BG10" s="21"/>
+      <c r="BH10" s="21"/>
+      <c r="BI10" s="21"/>
+      <c r="BJ10" s="21"/>
+      <c r="BK10" s="21"/>
+      <c r="BL10" s="21"/>
+      <c r="BM10" s="21"/>
+      <c r="BN10" s="21"/>
+      <c r="BO10" s="21"/>
+      <c r="BP10" s="21"/>
+      <c r="BQ10" s="21"/>
+      <c r="BR10" s="21"/>
+      <c r="BS10" s="21"/>
+      <c r="BT10" s="21"/>
+      <c r="BU10" s="21"/>
+      <c r="BV10" s="21"/>
+      <c r="BW10" s="21"/>
+      <c r="BX10" s="21"/>
+      <c r="BY10" s="21"/>
+      <c r="BZ10" s="21"/>
+      <c r="CA10" s="21"/>
+      <c r="CB10" s="21"/>
+      <c r="CC10" s="21"/>
+      <c r="CD10" s="21"/>
+      <c r="CE10" s="21"/>
+      <c r="CF10" s="21"/>
+      <c r="CG10" s="21"/>
+      <c r="CH10" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="CI10" s="23"/>
+      <c r="CJ10" s="23"/>
+      <c r="CK10" s="23"/>
+      <c r="CL10" s="23"/>
+      <c r="CM10" s="23"/>
+      <c r="CN10" s="23"/>
+      <c r="CO10" s="23" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="J11" s="22"/>
+      <c r="K11" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="23"/>
+      <c r="AB11" s="23"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="23"/>
+      <c r="AE11" s="23"/>
+      <c r="AF11" s="23"/>
+      <c r="AG11" s="23"/>
+      <c r="AH11" s="23"/>
+      <c r="AI11" s="23"/>
+      <c r="AJ11" s="23"/>
+      <c r="AK11" s="23"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="23"/>
+      <c r="AN11" s="21"/>
+      <c r="AO11" s="21"/>
+      <c r="AP11" s="21"/>
+      <c r="AQ11" s="21"/>
+      <c r="AR11" s="21"/>
+      <c r="AS11" s="21"/>
+      <c r="AT11" s="21"/>
+      <c r="AU11" s="21"/>
+      <c r="AV11" s="21"/>
+      <c r="AW11" s="21"/>
+      <c r="AX11" s="21"/>
+      <c r="AY11" s="21"/>
+      <c r="AZ11" s="21"/>
+      <c r="BA11" s="21"/>
+      <c r="BB11" s="21"/>
+      <c r="BC11" s="21"/>
+      <c r="BD11" s="21"/>
+      <c r="BE11" s="23"/>
+      <c r="BF11" s="21"/>
+      <c r="BG11" s="21"/>
+      <c r="BH11" s="21"/>
+      <c r="BI11" s="21"/>
+      <c r="BJ11" s="21"/>
+      <c r="BK11" s="21"/>
+      <c r="BL11" s="21"/>
+      <c r="BM11" s="21"/>
+      <c r="BN11" s="21"/>
+      <c r="BO11" s="21"/>
+      <c r="BP11" s="21"/>
+      <c r="BQ11" s="21"/>
+      <c r="BR11" s="21"/>
+      <c r="BS11" s="21"/>
+      <c r="BT11" s="21"/>
+      <c r="BU11" s="21"/>
+      <c r="BV11" s="21"/>
+      <c r="BW11" s="21"/>
+      <c r="BX11" s="21"/>
+      <c r="BY11" s="21"/>
+      <c r="BZ11" s="21"/>
+      <c r="CA11" s="21"/>
+      <c r="CB11" s="21"/>
+      <c r="CC11" s="21"/>
+      <c r="CD11" s="21"/>
+      <c r="CE11" s="21"/>
+      <c r="CF11" s="21"/>
+      <c r="CG11" s="21"/>
+      <c r="CH11" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="CI11" s="23"/>
+      <c r="CJ11" s="23"/>
+      <c r="CK11" s="23"/>
+      <c r="CL11" s="23"/>
+      <c r="CM11" s="23"/>
+      <c r="CN11" s="23"/>
+      <c r="CO11" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="H12" s="21"/>
+      <c r="I12" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="J12" s="22"/>
+      <c r="K12" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
+      <c r="AA12" s="23"/>
+      <c r="AB12" s="23"/>
+      <c r="AC12" s="23"/>
+      <c r="AD12" s="23"/>
+      <c r="AE12" s="23"/>
+      <c r="AF12" s="23"/>
+      <c r="AG12" s="23"/>
+      <c r="AH12" s="23"/>
+      <c r="AI12" s="23"/>
+      <c r="AJ12" s="23"/>
+      <c r="AK12" s="23"/>
+      <c r="AL12" s="23"/>
+      <c r="AM12" s="23"/>
+      <c r="AN12" s="21"/>
+      <c r="AO12" s="21"/>
+      <c r="AP12" s="21"/>
+      <c r="AQ12" s="21"/>
+      <c r="AR12" s="21"/>
+      <c r="AS12" s="21"/>
+      <c r="AT12" s="21"/>
+      <c r="AU12" s="21"/>
+      <c r="AV12" s="21"/>
+      <c r="AW12" s="21"/>
+      <c r="AX12" s="21"/>
+      <c r="AY12" s="21"/>
+      <c r="AZ12" s="21"/>
+      <c r="BA12" s="21"/>
+      <c r="BB12" s="21"/>
+      <c r="BC12" s="21"/>
+      <c r="BD12" s="21"/>
+      <c r="BE12" s="23"/>
+      <c r="BF12" s="21"/>
+      <c r="BG12" s="21"/>
+      <c r="BH12" s="21"/>
+      <c r="BI12" s="21"/>
+      <c r="BJ12" s="21"/>
+      <c r="BK12" s="21"/>
+      <c r="BL12" s="21"/>
+      <c r="BM12" s="21"/>
+      <c r="BN12" s="21"/>
+      <c r="BO12" s="21"/>
+      <c r="BP12" s="21"/>
+      <c r="BQ12" s="21"/>
+      <c r="BR12" s="21"/>
+      <c r="BS12" s="21"/>
+      <c r="BT12" s="21"/>
+      <c r="BU12" s="21"/>
+      <c r="BV12" s="21"/>
+      <c r="BW12" s="21"/>
+      <c r="BX12" s="21"/>
+      <c r="BY12" s="21"/>
+      <c r="BZ12" s="21"/>
+      <c r="CA12" s="21"/>
+      <c r="CB12" s="21"/>
+      <c r="CC12" s="21"/>
+      <c r="CD12" s="21"/>
+      <c r="CE12" s="21"/>
+      <c r="CF12" s="21"/>
+      <c r="CG12" s="21"/>
+      <c r="CH12" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="CI12" s="23"/>
+      <c r="CJ12" s="23"/>
+      <c r="CK12" s="23"/>
+      <c r="CL12" s="23"/>
+      <c r="CM12" s="23"/>
+      <c r="CN12" s="23"/>
+      <c r="CO12" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="J13" s="22"/>
+      <c r="K13" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="23"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
+      <c r="AC13" s="23"/>
+      <c r="AD13" s="23"/>
+      <c r="AE13" s="23"/>
+      <c r="AF13" s="23"/>
+      <c r="AG13" s="23"/>
+      <c r="AH13" s="23"/>
+      <c r="AI13" s="23"/>
+      <c r="AJ13" s="23"/>
+      <c r="AK13" s="23"/>
+      <c r="AL13" s="23"/>
+      <c r="AM13" s="23"/>
+      <c r="AN13" s="21"/>
+      <c r="AO13" s="21"/>
+      <c r="AP13" s="21"/>
+      <c r="AQ13" s="21"/>
+      <c r="AR13" s="21"/>
+      <c r="AS13" s="21"/>
+      <c r="AT13" s="21"/>
+      <c r="AU13" s="21"/>
+      <c r="AV13" s="21"/>
+      <c r="AW13" s="21"/>
+      <c r="AX13" s="21"/>
+      <c r="AY13" s="21"/>
+      <c r="AZ13" s="21"/>
+      <c r="BA13" s="21"/>
+      <c r="BB13" s="21"/>
+      <c r="BC13" s="21"/>
+      <c r="BD13" s="21"/>
+      <c r="BE13" s="23"/>
+      <c r="BF13" s="21"/>
+      <c r="BG13" s="21"/>
+      <c r="BH13" s="21"/>
+      <c r="BI13" s="21"/>
+      <c r="BJ13" s="21"/>
+      <c r="BK13" s="21"/>
+      <c r="BL13" s="21"/>
+      <c r="BM13" s="21"/>
+      <c r="BN13" s="21"/>
+      <c r="BO13" s="21"/>
+      <c r="BP13" s="21"/>
+      <c r="BQ13" s="21"/>
+      <c r="BR13" s="21"/>
+      <c r="BS13" s="21"/>
+      <c r="BT13" s="21"/>
+      <c r="BU13" s="21"/>
+      <c r="BV13" s="21"/>
+      <c r="BW13" s="21"/>
+      <c r="BX13" s="21"/>
+      <c r="BY13" s="21"/>
+      <c r="BZ13" s="21"/>
+      <c r="CA13" s="21"/>
+      <c r="CB13" s="21"/>
+      <c r="CC13" s="21"/>
+      <c r="CD13" s="21"/>
+      <c r="CE13" s="21"/>
+      <c r="CF13" s="21"/>
+      <c r="CG13" s="21"/>
+      <c r="CH13" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="CI13" s="23"/>
+      <c r="CJ13" s="23"/>
+      <c r="CK13" s="23"/>
+      <c r="CL13" s="23"/>
+      <c r="CM13" s="23"/>
+      <c r="CN13" s="23"/>
+      <c r="CO13" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="H14" s="21"/>
+      <c r="I14" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="J14" s="22"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="M14" s="22"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="23"/>
+      <c r="AA14" s="23"/>
+      <c r="AB14" s="23"/>
+      <c r="AC14" s="23"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="23"/>
+      <c r="AF14" s="23"/>
+      <c r="AG14" s="23"/>
+      <c r="AH14" s="23"/>
+      <c r="AI14" s="23"/>
+      <c r="AJ14" s="23"/>
+      <c r="AK14" s="23"/>
+      <c r="AL14" s="23"/>
+      <c r="AM14" s="23"/>
+      <c r="AN14" s="21"/>
+      <c r="AO14" s="21"/>
+      <c r="AP14" s="21"/>
+      <c r="AQ14" s="21"/>
+      <c r="AR14" s="21"/>
+      <c r="AS14" s="21"/>
+      <c r="AT14" s="21"/>
+      <c r="AU14" s="21"/>
+      <c r="AV14" s="21"/>
+      <c r="AW14" s="21"/>
+      <c r="AX14" s="21"/>
+      <c r="AY14" s="21"/>
+      <c r="AZ14" s="21"/>
+      <c r="BA14" s="21"/>
+      <c r="BB14" s="21"/>
+      <c r="BC14" s="21"/>
+      <c r="BD14" s="21"/>
+      <c r="BE14" s="23"/>
+      <c r="BF14" s="21"/>
+      <c r="BG14" s="21"/>
+      <c r="BH14" s="21"/>
+      <c r="BI14" s="21"/>
+      <c r="BJ14" s="21"/>
+      <c r="BK14" s="21"/>
+      <c r="BL14" s="21"/>
+      <c r="BM14" s="21"/>
+      <c r="BN14" s="21"/>
+      <c r="BO14" s="21"/>
+      <c r="BP14" s="21"/>
+      <c r="BQ14" s="21"/>
+      <c r="BR14" s="21"/>
+      <c r="BS14" s="21"/>
+      <c r="BT14" s="21"/>
+      <c r="BU14" s="21"/>
+      <c r="BV14" s="21"/>
+      <c r="BW14" s="21"/>
+      <c r="BX14" s="21"/>
+      <c r="BY14" s="21"/>
+      <c r="BZ14" s="21"/>
+      <c r="CA14" s="21"/>
+      <c r="CB14" s="21"/>
+      <c r="CC14" s="21"/>
+      <c r="CD14" s="21"/>
+      <c r="CE14" s="21"/>
+      <c r="CF14" s="21"/>
+      <c r="CG14" s="21"/>
+      <c r="CH14" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="CI14" s="23"/>
+      <c r="CJ14" s="23"/>
+      <c r="CK14" s="23"/>
+      <c r="CL14" s="23"/>
+      <c r="CM14" s="23"/>
+      <c r="CN14" s="23"/>
+      <c r="CO14" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="N15" s="21"/>
+      <c r="O15" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q15" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="R15" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="S15" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="T15" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="U15" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23"/>
+      <c r="AB15" s="23"/>
+      <c r="AC15" s="23"/>
+      <c r="AD15" s="23"/>
+      <c r="AE15" s="23"/>
+      <c r="AF15" s="23"/>
+      <c r="AG15" s="23"/>
+      <c r="AH15" s="23"/>
+      <c r="AI15" s="23"/>
+      <c r="AJ15" s="23"/>
+      <c r="AK15" s="23"/>
+      <c r="AL15" s="23"/>
+      <c r="AM15" s="23"/>
+      <c r="AN15" s="21"/>
+      <c r="AO15" s="21"/>
+      <c r="AP15" s="21"/>
+      <c r="AQ15" s="21"/>
+      <c r="AR15" s="21"/>
+      <c r="AS15" s="21"/>
+      <c r="AT15" s="21"/>
+      <c r="AU15" s="21"/>
+      <c r="AV15" s="21"/>
+      <c r="AW15" s="21"/>
+      <c r="AX15" s="21"/>
+      <c r="AY15" s="21"/>
+      <c r="AZ15" s="21"/>
+      <c r="BA15" s="21"/>
+      <c r="BB15" s="21"/>
+      <c r="BC15" s="21"/>
+      <c r="BD15" s="21"/>
+      <c r="BE15" s="23"/>
+      <c r="BF15" s="21"/>
+      <c r="BG15" s="21"/>
+      <c r="BH15" s="21"/>
+      <c r="BI15" s="21"/>
+      <c r="BJ15" s="21"/>
+      <c r="BK15" s="21"/>
+      <c r="BL15" s="21"/>
+      <c r="BM15" s="21"/>
+      <c r="BN15" s="21"/>
+      <c r="BO15" s="21"/>
+      <c r="BP15" s="21"/>
+      <c r="BQ15" s="21"/>
+      <c r="BR15" s="21"/>
+      <c r="BS15" s="21"/>
+      <c r="BT15" s="21"/>
+      <c r="BU15" s="21"/>
+      <c r="BV15" s="21"/>
+      <c r="BW15" s="21"/>
+      <c r="BX15" s="21"/>
+      <c r="BY15" s="21"/>
+      <c r="BZ15" s="21"/>
+      <c r="CA15" s="21"/>
+      <c r="CB15" s="21"/>
+      <c r="CC15" s="21"/>
+      <c r="CD15" s="21"/>
+      <c r="CE15" s="21"/>
+      <c r="CF15" s="21"/>
+      <c r="CG15" s="21"/>
+      <c r="CH15" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="CI15" s="23"/>
+      <c r="CJ15" s="23"/>
+      <c r="CK15" s="23"/>
+      <c r="CL15" s="23"/>
+      <c r="CM15" s="23"/>
+      <c r="CN15" s="23"/>
+      <c r="CO15" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="21" t="s">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
-      <c r="AM11" s="1"/>
-      <c r="AN11" s="1"/>
-      <c r="AO11" s="1"/>
-      <c r="AP11" s="1"/>
-      <c r="AQ11" s="1"/>
-      <c r="AR11" s="1"/>
-      <c r="AS11" s="1"/>
-      <c r="AT11" s="17" t="s">
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="AU11" s="1" t="s">
+      <c r="AU16" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="AV11" s="1"/>
-      <c r="AW11" s="1"/>
-      <c r="AX11" s="1"/>
-      <c r="AY11" s="1"/>
-      <c r="AZ11" s="1"/>
-      <c r="BA11" s="1"/>
-      <c r="BB11" s="1"/>
-      <c r="BC11" s="1"/>
-      <c r="BD11" s="1"/>
-      <c r="BE11" s="1"/>
-      <c r="BF11" s="1"/>
-      <c r="BG11" s="1"/>
-      <c r="BH11" s="1"/>
-      <c r="BI11" s="1"/>
-      <c r="BJ11" s="1"/>
-      <c r="BK11" s="1"/>
-      <c r="BL11" s="1"/>
-      <c r="BM11" s="1"/>
-      <c r="BN11" s="1"/>
-      <c r="BO11" s="1"/>
-      <c r="BP11" s="1"/>
-      <c r="BQ11" s="1"/>
-      <c r="BR11" s="1"/>
-      <c r="BS11" s="1"/>
-      <c r="BT11" s="1"/>
-      <c r="BU11" s="1"/>
-      <c r="BV11" s="1"/>
-      <c r="BW11" s="1"/>
-      <c r="BX11" s="1"/>
-      <c r="BY11" s="1"/>
-      <c r="BZ11" s="1"/>
-      <c r="CA11" s="1"/>
-      <c r="CB11" s="1"/>
-      <c r="CC11" s="1"/>
-      <c r="CD11" s="1"/>
-      <c r="CE11" s="1"/>
-      <c r="CF11" s="1"/>
-      <c r="CG11" s="1"/>
-      <c r="CH11" s="11">
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
+      <c r="BA16" s="1"/>
+      <c r="BB16" s="1"/>
+      <c r="BC16" s="1"/>
+      <c r="BD16" s="1"/>
+      <c r="BE16" s="1"/>
+      <c r="BF16" s="1"/>
+      <c r="BG16" s="1"/>
+      <c r="BH16" s="1"/>
+      <c r="BI16" s="1"/>
+      <c r="BJ16" s="1"/>
+      <c r="BK16" s="1"/>
+      <c r="BL16" s="1"/>
+      <c r="BM16" s="1"/>
+      <c r="BN16" s="1"/>
+      <c r="BO16" s="1"/>
+      <c r="BP16" s="1"/>
+      <c r="BQ16" s="1"/>
+      <c r="BR16" s="1"/>
+      <c r="BS16" s="1"/>
+      <c r="BT16" s="1"/>
+      <c r="BU16" s="1"/>
+      <c r="BV16" s="1"/>
+      <c r="BW16" s="1"/>
+      <c r="BX16" s="1"/>
+      <c r="BY16" s="1"/>
+      <c r="BZ16" s="1"/>
+      <c r="CA16" s="1"/>
+      <c r="CB16" s="1"/>
+      <c r="CC16" s="1"/>
+      <c r="CD16" s="1"/>
+      <c r="CE16" s="1"/>
+      <c r="CF16" s="1"/>
+      <c r="CG16" s="1"/>
+      <c r="CH16" s="11">
         <v>91</v>
       </c>
-      <c r="CI11" s="1"/>
-      <c r="CJ11" s="1"/>
-      <c r="CK11" s="1"/>
-      <c r="CL11" s="1"/>
-      <c r="CM11" s="1"/>
-      <c r="CN11" s="1" t="s">
+      <c r="CI16" s="1"/>
+      <c r="CJ16" s="1"/>
+      <c r="CK16" s="1"/>
+      <c r="CL16" s="1"/>
+      <c r="CM16" s="1"/>
+      <c r="CN16" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="CO16" s="1">
+        <f>DATE(2021,1,28)</f>
+        <v>44224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AU17" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="1"/>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="1"/>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="1"/>
+      <c r="BC17" s="1"/>
+      <c r="BD17" s="1"/>
+      <c r="BE17" s="1"/>
+      <c r="BF17" s="1"/>
+      <c r="BG17" s="1"/>
+      <c r="BH17" s="1"/>
+      <c r="BI17" s="1"/>
+      <c r="BJ17" s="1"/>
+      <c r="BK17" s="1"/>
+      <c r="BL17" s="1"/>
+      <c r="BM17" s="1"/>
+      <c r="BN17" s="1"/>
+      <c r="BO17" s="1"/>
+      <c r="BP17" s="1"/>
+      <c r="BQ17" s="1"/>
+      <c r="BR17" s="1"/>
+      <c r="BS17" s="1"/>
+      <c r="BT17" s="1"/>
+      <c r="BU17" s="1"/>
+      <c r="BV17" s="1"/>
+      <c r="BW17" s="1"/>
+      <c r="BX17" s="1"/>
+      <c r="BY17" s="1"/>
+      <c r="BZ17" s="1"/>
+      <c r="CA17" s="1"/>
+      <c r="CB17" s="1"/>
+      <c r="CC17" s="1"/>
+      <c r="CD17" s="1"/>
+      <c r="CE17" s="1"/>
+      <c r="CF17" s="1"/>
+      <c r="CG17" s="1"/>
+      <c r="CH17" s="11">
+        <v>91</v>
+      </c>
+      <c r="CI17" s="1"/>
+      <c r="CJ17" s="1"/>
+      <c r="CK17" s="1"/>
+      <c r="CL17" s="1"/>
+      <c r="CM17" s="1"/>
+      <c r="CN17" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="CO17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
engagement report case added in k12
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104FEAB4-B3EB-4737-9513-3CEF1A9C8458}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C52F793-3447-420C-8B01-14D4364D45F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="250">
   <si>
     <t>Environment</t>
   </si>
@@ -778,9 +778,6 @@
   </si>
   <si>
     <t>10</t>
-  </si>
-  <si>
-    <t>Q 3</t>
   </si>
   <si>
     <t>Dar report</t>
@@ -836,25 +833,34 @@
     <t>Teacher/Staff</t>
   </si>
   <si>
-    <t>Q 9</t>
-  </si>
-  <si>
-    <t>Q 10</t>
-  </si>
-  <si>
     <t>Subject Taught</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>Department</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
-    <t>Not showing email to pop up on generated report</t>
+    <t>School Site,Subject Taught,Department,Grade Level,Gender</t>
+  </si>
+  <si>
+    <t>199</t>
+  </si>
+  <si>
+    <t>Engagement Exe check</t>
+  </si>
+  <si>
+    <t>Q 2</t>
+  </si>
+  <si>
+    <t>Q 5</t>
+  </si>
+  <si>
+    <t>Q 1</t>
+  </si>
+  <si>
+    <t>4,5,6,7,8</t>
   </si>
 </sst>
 </file>
@@ -1490,8 +1496,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CO16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2880,7 +2886,7 @@
       <c r="U10" s="22"/>
       <c r="V10" s="22"/>
       <c r="W10" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X10" s="22"/>
       <c r="Y10" s="22"/>
@@ -2999,7 +3005,7 @@
       <c r="U11" s="22"/>
       <c r="V11" s="22"/>
       <c r="W11" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X11" s="22"/>
       <c r="Y11" s="22"/>
@@ -3118,7 +3124,7 @@
       <c r="U12" s="22"/>
       <c r="V12" s="22"/>
       <c r="W12" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X12" s="22"/>
       <c r="Y12" s="22"/>
@@ -3237,7 +3243,7 @@
       <c r="U13" s="22"/>
       <c r="V13" s="22"/>
       <c r="W13" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X13" s="22"/>
       <c r="Y13" s="22"/>
@@ -3356,7 +3362,7 @@
       <c r="U14" s="22"/>
       <c r="V14" s="22"/>
       <c r="W14" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X14" s="22"/>
       <c r="Y14" s="22"/>
@@ -3456,32 +3462,30 @@
         <v>221</v>
       </c>
       <c r="H15" s="20"/>
-      <c r="I15" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="J15" s="21" t="s">
-        <v>247</v>
-      </c>
+      <c r="I15" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="J15" s="21"/>
       <c r="K15" s="20" t="s">
         <v>222</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O15" s="22" t="s">
         <v>231</v>
       </c>
       <c r="P15" s="20" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="Q15" s="22" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="R15" s="22" t="s">
         <v>223</v>
@@ -3490,16 +3494,16 @@
         <v>224</v>
       </c>
       <c r="T15" s="20" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="U15" s="22" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="V15" s="22" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="W15" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X15" s="22"/>
       <c r="Y15" s="22"/>
@@ -3564,7 +3568,7 @@
       <c r="CF15" s="20"/>
       <c r="CG15" s="20"/>
       <c r="CH15" s="22" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="CI15" s="22"/>
       <c r="CJ15" s="22"/>
@@ -3573,7 +3577,7 @@
       <c r="CM15" s="22"/>
       <c r="CN15" s="22"/>
       <c r="CO15" s="22" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:93" x14ac:dyDescent="0.25">
@@ -3593,10 +3597,10 @@
         <v>201</v>
       </c>
       <c r="F16" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="G16" s="20" t="s">
         <v>233</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>234</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="17" t="s">
@@ -3607,20 +3611,20 @@
         <v>183</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N16" s="20"/>
       <c r="O16" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q16" s="22" t="s">
         <v>223</v>
       </c>
       <c r="R16" s="22" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="S16" s="22" t="s">
         <v>224</v>
@@ -3633,7 +3637,7 @@
       </c>
       <c r="V16" s="22"/>
       <c r="W16" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="X16" s="22"/>
       <c r="Y16" s="22"/>
@@ -3698,7 +3702,7 @@
       <c r="CF16" s="20"/>
       <c r="CG16" s="20"/>
       <c r="CH16" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="CI16" s="22"/>
       <c r="CJ16" s="22"/>

</xml_diff>

<commit_message>
Omni segmentation exe and PDF export type is added
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C6CD74-B0E4-47E2-BA3A-B303805244F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338DD9C8-FF19-42D7-9434-53DE47985B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="0" windowWidth="15150" windowHeight="10920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="263">
   <si>
     <t>Environment</t>
   </si>
@@ -848,12 +848,6 @@
     <t>Engagement Exe check</t>
   </si>
   <si>
-    <t>ggolatkar@zarca.com</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>Data Import</t>
   </si>
   <si>
@@ -879,14 +873,31 @@
   </si>
   <si>
     <t>Data Export</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The excel was not downloaded.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Overall Score Data Table not present on page.</t>
+  </si>
+  <si>
+    <t>kchavan@zarca.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Email Engagement Report not present on page.</t>
+  </si>
+  <si>
+    <t>Q 5. CB: Which types of meat do you like?</t>
+  </si>
+  <si>
+    <t>DP - Segment Group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -912,6 +923,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -931,19 +943,8 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -968,48 +969,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -1090,7 +1056,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1121,14 +1087,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1424,8 +1385,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,9 +1426,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,10 +1469,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1572,13 +1533,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
@@ -1600,30 +1561,30 @@
   <dimension ref="A1:CO19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="42.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="92" max="93" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="92" max="93" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:93" x14ac:dyDescent="0.25">
@@ -1930,7 +1891,7 @@
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J2" s="13"/>
@@ -2043,7 +2004,7 @@
       <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J3" s="13"/>
@@ -2234,7 +2195,7 @@
       <c r="H4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J4" s="13"/>
@@ -2331,10 +2292,10 @@
       <c r="CM4" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="CN4" s="33" t="s">
+      <c r="CN4" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="CO4" s="33"/>
+      <c r="CO4" s="30"/>
     </row>
     <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2359,7 +2320,7 @@
       <c r="H5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J5" s="12"/>
@@ -2484,7 +2445,7 @@
       <c r="H6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J6" s="13"/>
@@ -2599,10 +2560,12 @@
       <c r="H7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="J7" s="12" t="s">
+        <v>257</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -2716,7 +2679,7 @@
       <c r="H8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J8" s="13"/>
@@ -2833,7 +2796,7 @@
       <c r="H9" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J9" s="1"/>
@@ -2940,7 +2903,7 @@
         <v>188</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>15</v>
@@ -2958,7 +2921,7 @@
         <v>193</v>
       </c>
       <c r="H10" s="16"/>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J10" s="17"/>
@@ -2968,8 +2931,12 @@
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
       <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
+      <c r="O10" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>261</v>
+      </c>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
@@ -2977,7 +2944,7 @@
       <c r="U10" s="18"/>
       <c r="V10" s="18"/>
       <c r="W10" s="29" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
@@ -3077,7 +3044,7 @@
         <v>196</v>
       </c>
       <c r="H11" s="16"/>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J11" s="17"/>
@@ -3096,7 +3063,7 @@
       <c r="U11" s="18"/>
       <c r="V11" s="18"/>
       <c r="W11" s="29" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
@@ -3196,7 +3163,7 @@
         <v>200</v>
       </c>
       <c r="H12" s="16"/>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J12" s="17"/>
@@ -3215,7 +3182,7 @@
       <c r="U12" s="18"/>
       <c r="V12" s="18"/>
       <c r="W12" s="29" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
@@ -3315,7 +3282,7 @@
         <v>204</v>
       </c>
       <c r="H13" s="16"/>
-      <c r="I13" s="36" t="s">
+      <c r="I13" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J13" s="17"/>
@@ -3334,7 +3301,7 @@
       <c r="U13" s="18"/>
       <c r="V13" s="18"/>
       <c r="W13" s="29" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
@@ -3434,7 +3401,7 @@
         <v>208</v>
       </c>
       <c r="H14" s="16"/>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J14" s="17"/>
@@ -3453,7 +3420,7 @@
       <c r="U14" s="18"/>
       <c r="V14" s="18"/>
       <c r="W14" s="29" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
@@ -3535,7 +3502,7 @@
         <v>209</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>15</v>
@@ -3553,10 +3520,12 @@
         <v>211</v>
       </c>
       <c r="H15" s="26"/>
-      <c r="I15" s="36" t="s">
-        <v>190</v>
-      </c>
-      <c r="J15" s="27"/>
+      <c r="I15" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>260</v>
+      </c>
       <c r="K15" s="26" t="s">
         <v>212</v>
       </c>
@@ -3594,7 +3563,7 @@
         <v>245</v>
       </c>
       <c r="W15" s="29" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="X15" s="28"/>
       <c r="Y15" s="28"/>
@@ -3676,7 +3645,7 @@
         <v>217</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>15</v>
@@ -3694,10 +3663,12 @@
         <v>233</v>
       </c>
       <c r="H16" s="22"/>
-      <c r="I16" s="36" t="s">
-        <v>190</v>
-      </c>
-      <c r="J16" s="21"/>
+      <c r="I16" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>258</v>
+      </c>
       <c r="K16" s="22" t="s">
         <v>179</v>
       </c>
@@ -3729,7 +3700,7 @@
       </c>
       <c r="V16" s="24"/>
       <c r="W16" s="29" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="X16" s="24"/>
       <c r="Y16" s="24"/>
@@ -3829,7 +3800,7 @@
       <c r="H17" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I17" s="36" t="s">
+      <c r="I17" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J17" s="13"/>
@@ -3926,17 +3897,17 @@
       <c r="CM17" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="CN17" s="33" t="s">
+      <c r="CN17" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="CO17" s="33"/>
+      <c r="CO17" s="30"/>
     </row>
     <row r="18" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -3945,15 +3916,15 @@
         <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="34" t="s">
-        <v>229</v>
+      <c r="I18" s="32" t="s">
+        <v>190</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="1"/>
@@ -3992,7 +3963,7 @@
       <c r="AR18" s="11"/>
       <c r="AS18" s="11"/>
       <c r="AT18" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AU18" s="11"/>
       <c r="AV18" s="11"/>
@@ -4038,20 +4009,20 @@
       </c>
       <c r="CI18" s="14"/>
       <c r="CJ18" s="15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="CK18" s="12"/>
       <c r="CL18" s="12"/>
       <c r="CM18" s="12"/>
-      <c r="CN18" s="33"/>
-      <c r="CO18" s="33"/>
+      <c r="CN18" s="30"/>
+      <c r="CO18" s="30"/>
     </row>
     <row r="19" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -4060,15 +4031,15 @@
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="34" t="s">
-        <v>229</v>
+      <c r="I19" s="32" t="s">
+        <v>190</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="1"/>
@@ -4109,7 +4080,7 @@
       <c r="AR19" s="11"/>
       <c r="AS19" s="11"/>
       <c r="AT19" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AU19" s="11"/>
       <c r="AV19" s="11"/>
@@ -4158,18 +4129,17 @@
       <c r="CK19" s="12"/>
       <c r="CL19" s="12"/>
       <c r="CM19" s="12"/>
-      <c r="CN19" s="33"/>
-      <c r="CO19" s="33"/>
+      <c r="CN19" s="30"/>
+      <c r="CO19" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
     <hyperlink ref="W10" r:id="rId2" xr:uid="{1A3A3DAA-C543-4D04-861C-36D2AA5A4FAA}"/>
-    <hyperlink ref="W11:W15" r:id="rId3" display="ggolatkar@zarca.com" xr:uid="{F8CAF336-4B49-413C-B84B-31D28BAB683A}"/>
-    <hyperlink ref="W16" r:id="rId4" xr:uid="{38206B95-127E-4BF7-A610-3AB1C32EE781}"/>
+    <hyperlink ref="W11:W16" r:id="rId3" display="kchavan@zarca.com" xr:uid="{55B2641E-366D-4B03-AD07-8497F5A731DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OMNI EXE added and PDF export included with git ignore changes
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C6CD74-B0E4-47E2-BA3A-B303805244F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6EC67E-F2DA-42CA-8666-F881A23A1AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="600" windowWidth="15150" windowHeight="10920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="262">
   <si>
     <t>Environment</t>
   </si>
@@ -848,12 +848,6 @@
     <t>Engagement Exe check</t>
   </si>
   <si>
-    <t>ggolatkar@zarca.com</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>Data Import</t>
   </si>
   <si>
@@ -879,14 +873,28 @@
   </si>
   <si>
     <t>Data Export</t>
+  </si>
+  <si>
+    <t>kchavan@zarca.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ranking Button not present on page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Email Engagement Report not present on page.</t>
+  </si>
+  <si>
+    <t>DP - Segment Group</t>
+  </si>
+  <si>
+    <t>Q 5. CB: Which types of meat do you like?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -931,19 +939,8 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -968,43 +965,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
       </patternFill>
     </fill>
     <fill>
@@ -1081,7 +1048,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
@@ -1089,8 +1056,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1121,23 +1095,26 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="9" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="14">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{E0C9F20A-3C63-41E3-B488-667155B99753}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="11" xr:uid="{266E5B1D-F7E5-4947-9EE7-36ACB7FB4844}"/>
+    <cellStyle name="Hyperlink 3" xfId="8" xr:uid="{7545D0E5-C627-4B1D-9EE0-A5A30E1492F0}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{BEFE91A1-6694-4EFC-B4C7-79AC9427A142}"/>
+    <cellStyle name="Normal 2 2" xfId="9" xr:uid="{22EE6E41-3A88-4E00-9A70-1CEAFA4C0A47}"/>
     <cellStyle name="Normal 3" xfId="5" xr:uid="{33784278-FC36-4C89-A3F0-5F104988CE08}"/>
+    <cellStyle name="Normal 3 2" xfId="12" xr:uid="{E3F897AF-A356-4BEA-AB8F-08EF37734491}"/>
     <cellStyle name="Normal 4" xfId="3" xr:uid="{E3D7501D-72D4-41B1-89B8-6CC3B051C17C}"/>
+    <cellStyle name="Normal 4 2" xfId="10" xr:uid="{2A402E83-0D9F-4A8E-9534-92C03218AF6A}"/>
     <cellStyle name="Normal 5" xfId="6" xr:uid="{CA8A5EF5-7DD1-4FF3-9C16-F3ECD1AB37FA}"/>
+    <cellStyle name="Normal 5 2" xfId="13" xr:uid="{09540B07-B51B-482E-9F69-52483B3D8E9D}"/>
+    <cellStyle name="Normal 6" xfId="7" xr:uid="{CE04887E-3E3A-421D-8E2D-455F57AF8A48}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1424,8 +1401,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,9 +1442,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,10 +1485,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1572,13 +1549,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>3</v>
@@ -1599,31 +1576,31 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CO19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10:P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="42.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="92" max="93" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="92" max="93" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:93" x14ac:dyDescent="0.25">
@@ -1930,7 +1907,7 @@
       <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J2" s="13"/>
@@ -2025,7 +2002,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -2043,10 +2020,12 @@
       <c r="H3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>190</v>
-      </c>
-      <c r="J3" s="13"/>
+      <c r="I3" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>258</v>
+      </c>
       <c r="K3" s="1"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -2234,7 +2213,7 @@
       <c r="H4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J4" s="13"/>
@@ -2331,10 +2310,10 @@
       <c r="CM4" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="CN4" s="33" t="s">
+      <c r="CN4" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="CO4" s="33"/>
+      <c r="CO4" s="30"/>
     </row>
     <row r="5" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2359,7 +2338,7 @@
       <c r="H5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="36" t="s">
+      <c r="I5" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J5" s="12"/>
@@ -2484,7 +2463,7 @@
       <c r="H6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J6" s="13"/>
@@ -2599,7 +2578,7 @@
       <c r="H7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I7" s="36" t="s">
+      <c r="I7" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J7" s="12"/>
@@ -2716,7 +2695,7 @@
       <c r="H8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J8" s="13"/>
@@ -2833,7 +2812,7 @@
       <c r="H9" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J9" s="1"/>
@@ -2958,7 +2937,7 @@
         <v>193</v>
       </c>
       <c r="H10" s="16"/>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J10" s="17"/>
@@ -2968,8 +2947,12 @@
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
       <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
+      <c r="O10" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="P10" s="33" t="s">
+        <v>261</v>
+      </c>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
@@ -2977,7 +2960,7 @@
       <c r="U10" s="18"/>
       <c r="V10" s="18"/>
       <c r="W10" s="29" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="X10" s="18"/>
       <c r="Y10" s="18"/>
@@ -3077,7 +3060,7 @@
         <v>196</v>
       </c>
       <c r="H11" s="16"/>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J11" s="17"/>
@@ -3096,7 +3079,7 @@
       <c r="U11" s="18"/>
       <c r="V11" s="18"/>
       <c r="W11" s="29" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="X11" s="18"/>
       <c r="Y11" s="18"/>
@@ -3196,7 +3179,7 @@
         <v>200</v>
       </c>
       <c r="H12" s="16"/>
-      <c r="I12" s="36" t="s">
+      <c r="I12" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J12" s="17"/>
@@ -3215,7 +3198,7 @@
       <c r="U12" s="18"/>
       <c r="V12" s="18"/>
       <c r="W12" s="29" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="X12" s="18"/>
       <c r="Y12" s="18"/>
@@ -3315,7 +3298,7 @@
         <v>204</v>
       </c>
       <c r="H13" s="16"/>
-      <c r="I13" s="36" t="s">
+      <c r="I13" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J13" s="17"/>
@@ -3334,7 +3317,7 @@
       <c r="U13" s="18"/>
       <c r="V13" s="18"/>
       <c r="W13" s="29" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="X13" s="18"/>
       <c r="Y13" s="18"/>
@@ -3434,7 +3417,7 @@
         <v>208</v>
       </c>
       <c r="H14" s="16"/>
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J14" s="17"/>
@@ -3453,7 +3436,7 @@
       <c r="U14" s="18"/>
       <c r="V14" s="18"/>
       <c r="W14" s="29" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="X14" s="18"/>
       <c r="Y14" s="18"/>
@@ -3553,10 +3536,12 @@
         <v>211</v>
       </c>
       <c r="H15" s="26"/>
-      <c r="I15" s="36" t="s">
+      <c r="I15" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="J15" s="27"/>
+      <c r="J15" s="27" t="s">
+        <v>259</v>
+      </c>
       <c r="K15" s="26" t="s">
         <v>212</v>
       </c>
@@ -3594,7 +3579,7 @@
         <v>245</v>
       </c>
       <c r="W15" s="29" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="X15" s="28"/>
       <c r="Y15" s="28"/>
@@ -3694,7 +3679,7 @@
         <v>233</v>
       </c>
       <c r="H16" s="22"/>
-      <c r="I16" s="36" t="s">
+      <c r="I16" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J16" s="21"/>
@@ -3729,7 +3714,7 @@
       </c>
       <c r="V16" s="24"/>
       <c r="W16" s="29" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="X16" s="24"/>
       <c r="Y16" s="24"/>
@@ -3829,7 +3814,7 @@
       <c r="H17" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I17" s="36" t="s">
+      <c r="I17" s="32" t="s">
         <v>190</v>
       </c>
       <c r="J17" s="13"/>
@@ -3926,17 +3911,17 @@
       <c r="CM17" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="CN17" s="33" t="s">
+      <c r="CN17" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="CO17" s="33"/>
+      <c r="CO17" s="30"/>
     </row>
     <row r="18" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -3945,15 +3930,15 @@
         <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="34" t="s">
-        <v>229</v>
+      <c r="I18" s="32" t="s">
+        <v>190</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="1"/>
@@ -3992,7 +3977,7 @@
       <c r="AR18" s="11"/>
       <c r="AS18" s="11"/>
       <c r="AT18" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AU18" s="11"/>
       <c r="AV18" s="11"/>
@@ -4038,20 +4023,20 @@
       </c>
       <c r="CI18" s="14"/>
       <c r="CJ18" s="15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="CK18" s="12"/>
       <c r="CL18" s="12"/>
       <c r="CM18" s="12"/>
-      <c r="CN18" s="33"/>
-      <c r="CO18" s="33"/>
+      <c r="CN18" s="30"/>
+      <c r="CO18" s="30"/>
     </row>
     <row r="19" spans="1:93" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -4060,15 +4045,15 @@
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="34" t="s">
-        <v>229</v>
+      <c r="I19" s="32" t="s">
+        <v>190</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="1"/>
@@ -4109,7 +4094,7 @@
       <c r="AR19" s="11"/>
       <c r="AS19" s="11"/>
       <c r="AT19" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AU19" s="11"/>
       <c r="AV19" s="11"/>
@@ -4158,18 +4143,17 @@
       <c r="CK19" s="12"/>
       <c r="CL19" s="12"/>
       <c r="CM19" s="12"/>
-      <c r="CN19" s="33"/>
-      <c r="CO19" s="33"/>
+      <c r="CN19" s="30"/>
+      <c r="CO19" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
     <hyperlink ref="W10" r:id="rId2" xr:uid="{1A3A3DAA-C543-4D04-861C-36D2AA5A4FAA}"/>
-    <hyperlink ref="W11:W15" r:id="rId3" display="ggolatkar@zarca.com" xr:uid="{F8CAF336-4B49-413C-B84B-31D28BAB683A}"/>
-    <hyperlink ref="W16" r:id="rId4" xr:uid="{38206B95-127E-4BF7-A610-3AB1C32EE781}"/>
+    <hyperlink ref="W11:W16" r:id="rId3" display="kchavan@zarca.com" xr:uid="{398A7759-EEFF-4B0C-AEBC-AA147DE7CED1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Data in Excel File(Engage)
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="575">
   <si>
     <t>Environment</t>
   </si>
@@ -1866,17 +1866,24 @@
     <t>Your Voice Counts</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>This is a sample ranking question</t>
+  </si>
+  <si>
+    <t>This is a sample Date</t>
+  </si>
+  <si>
+    <t>This is a sample Horizontal Radio Question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1934,8 +1941,24 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1976,7 +1999,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -2088,7 +2141,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2140,8 +2193,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2444,8 +2501,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="42.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2485,9 +2542,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="60.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2528,10 +2585,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2633,33 +2690,33 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CV77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B2:B23"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="42.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="93" max="93" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="94" max="94" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="42.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="92" max="92" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="93" max="93" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="94" max="94" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:100" x14ac:dyDescent="0.25">
@@ -2987,7 +3044,7 @@
       <c r="H2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J2" s="13"/>
@@ -3107,7 +3164,7 @@
       <c r="H3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J3" s="13" t="s">
@@ -3307,7 +3364,7 @@
       <c r="H4" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J4" s="13"/>
@@ -3439,7 +3496,7 @@
       <c r="H5" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I5" s="48" t="s">
+      <c r="I5" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J5" s="12"/>
@@ -3571,7 +3628,7 @@
       <c r="H6" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J6" s="13"/>
@@ -3693,7 +3750,7 @@
       <c r="H7" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J7" s="12"/>
@@ -3817,7 +3874,7 @@
       <c r="H8" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J8" s="13"/>
@@ -3941,7 +3998,7 @@
       <c r="H9" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I9" s="48" t="s">
+      <c r="I9" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -4075,8 +4132,8 @@
         <v>192</v>
       </c>
       <c r="H10" s="16"/>
-      <c r="I10" s="47" t="s">
-        <v>571</v>
+      <c r="I10" s="51" t="s">
+        <v>189</v>
       </c>
       <c r="J10" s="17" t="s">
         <v>350</v>
@@ -4207,8 +4264,8 @@
         <v>195</v>
       </c>
       <c r="H11" s="16"/>
-      <c r="I11" s="46" t="s">
-        <v>572</v>
+      <c r="I11" s="51" t="s">
+        <v>189</v>
       </c>
       <c r="J11" s="17" t="s">
         <v>346</v>
@@ -4335,8 +4392,8 @@
         <v>199</v>
       </c>
       <c r="H12" s="16"/>
-      <c r="I12" s="46" t="s">
-        <v>572</v>
+      <c r="I12" s="51" t="s">
+        <v>189</v>
       </c>
       <c r="J12" s="17"/>
       <c r="K12" s="16" t="s">
@@ -4461,8 +4518,8 @@
         <v>203</v>
       </c>
       <c r="H13" s="16"/>
-      <c r="I13" s="46" t="s">
-        <v>572</v>
+      <c r="I13" s="51" t="s">
+        <v>189</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>346</v>
@@ -4589,8 +4646,8 @@
         <v>207</v>
       </c>
       <c r="H14" s="16"/>
-      <c r="I14" s="47" t="s">
-        <v>571</v>
+      <c r="I14" s="51" t="s">
+        <v>189</v>
       </c>
       <c r="J14" s="17" t="s">
         <v>346</v>
@@ -4717,8 +4774,8 @@
         <v>210</v>
       </c>
       <c r="H15" s="26"/>
-      <c r="I15" s="46" t="s">
-        <v>572</v>
+      <c r="I15" s="51" t="s">
+        <v>189</v>
       </c>
       <c r="J15" s="27" t="s">
         <v>255</v>
@@ -4867,8 +4924,8 @@
         <v>231</v>
       </c>
       <c r="H16" s="22"/>
-      <c r="I16" s="46" t="s">
-        <v>572</v>
+      <c r="I16" s="51" t="s">
+        <v>189</v>
       </c>
       <c r="J16" s="21"/>
       <c r="K16" s="22" t="s">
@@ -5009,7 +5066,7 @@
       <c r="H17" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I17" s="48" t="s">
+      <c r="I17" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J17" s="13" t="s">
@@ -5141,8 +5198,8 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="46" t="s">
-        <v>572</v>
+      <c r="I18" s="51" t="s">
+        <v>189</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="1"/>
@@ -5263,8 +5320,8 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="46" t="s">
-        <v>572</v>
+      <c r="I19" s="51" t="s">
+        <v>189</v>
       </c>
       <c r="J19" s="13" t="s">
         <v>347</v>
@@ -5387,7 +5444,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="48" t="s">
+      <c r="I20" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J20" s="13"/>
@@ -5513,7 +5570,7 @@
       <c r="H21" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="I21" s="48" t="s">
+      <c r="I21" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J21" s="1"/>
@@ -5639,7 +5696,7 @@
       <c r="H22" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I22" s="48" t="s">
+      <c r="I22" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J22" s="1"/>
@@ -5761,7 +5818,7 @@
       <c r="H23" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="I23" s="48" t="s">
+      <c r="I23" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J23" s="1"/>
@@ -5889,7 +5946,7 @@
       <c r="H24" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="I24" s="48" t="s">
+      <c r="I24" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J24" s="1"/>
@@ -6013,7 +6070,7 @@
       <c r="H25" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I25" s="48" t="s">
+      <c r="I25" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J25" s="1"/>
@@ -6137,7 +6194,7 @@
       <c r="H26" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I26" s="48" t="s">
+      <c r="I26" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J26" s="1"/>
@@ -6261,7 +6318,7 @@
       <c r="H27" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="I27" s="48" t="s">
+      <c r="I27" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J27" s="1"/>
@@ -6383,7 +6440,7 @@
       <c r="H28" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="I28" s="48" t="s">
+      <c r="I28" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J28" s="1"/>
@@ -6505,7 +6562,7 @@
       <c r="H29" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I29" s="48" t="s">
+      <c r="I29" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J29" s="1"/>
@@ -6629,7 +6686,7 @@
       <c r="H30" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="I30" s="48" t="s">
+      <c r="I30" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J30" s="1"/>
@@ -6755,7 +6812,7 @@
       <c r="H31" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="I31" s="48" t="s">
+      <c r="I31" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J31" s="1"/>
@@ -6881,7 +6938,7 @@
       <c r="H32" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="I32" s="48" t="s">
+      <c r="I32" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J32" s="1"/>
@@ -7005,7 +7062,7 @@
         <v>555</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="48" t="s">
+      <c r="I33" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J33" s="1"/>
@@ -7123,7 +7180,7 @@
         <v>518</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="48" t="s">
+      <c r="I34" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J34" s="1"/>
@@ -7253,7 +7310,7 @@
         <v>527</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="48" t="s">
+      <c r="I35" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J35" s="1"/>
@@ -7383,7 +7440,7 @@
         <v>530</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="48" t="s">
+      <c r="I36" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J36" s="1"/>
@@ -7513,7 +7570,7 @@
         <v>533</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="48" t="s">
+      <c r="I37" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J37" s="1"/>
@@ -7643,7 +7700,7 @@
         <v>536</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="48" t="s">
+      <c r="I38" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J38" s="1"/>
@@ -7773,7 +7830,7 @@
         <v>539</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="48" t="s">
+      <c r="I39" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J39" s="1"/>
@@ -7903,7 +7960,7 @@
         <v>542</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="48" t="s">
+      <c r="I40" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J40" s="1"/>
@@ -8033,7 +8090,7 @@
         <v>545</v>
       </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="48" t="s">
+      <c r="I41" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J41" s="1"/>
@@ -8099,7 +8156,9 @@
       <c r="BH41" s="1"/>
       <c r="BI41" s="1"/>
       <c r="BJ41" s="1"/>
-      <c r="BK41" s="1"/>
+      <c r="BK41" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL41" s="1"/>
       <c r="BM41" s="1"/>
       <c r="BN41" s="1"/>
@@ -8163,7 +8222,7 @@
         <v>548</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="48" t="s">
+      <c r="I42" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J42" s="1"/>
@@ -8225,7 +8284,9 @@
       <c r="BD42" s="1"/>
       <c r="BE42" s="1"/>
       <c r="BF42" s="1"/>
-      <c r="BG42" s="1"/>
+      <c r="BG42" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH42" s="1"/>
       <c r="BI42" s="1"/>
       <c r="BJ42" s="1"/>
@@ -8293,7 +8354,7 @@
         <v>551</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="48" t="s">
+      <c r="I43" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J43" s="1"/>
@@ -8373,7 +8434,9 @@
       <c r="BV43" s="1"/>
       <c r="BW43" s="1"/>
       <c r="BX43" s="1"/>
-      <c r="BY43" s="1"/>
+      <c r="BY43" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ43" s="1"/>
       <c r="CA43" s="1"/>
       <c r="CB43" s="1"/>
@@ -8423,7 +8486,7 @@
         <v>553</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="48" t="s">
+      <c r="I44" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J44" s="1"/>
@@ -8555,7 +8618,7 @@
       <c r="H45" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="I45" s="48" t="s">
+      <c r="I45" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J45" s="1"/>
@@ -8685,7 +8748,7 @@
       <c r="H46" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="I46" s="48" t="s">
+      <c r="I46" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J46" s="1"/>
@@ -8815,7 +8878,7 @@
       <c r="H47" s="36" t="s">
         <v>434</v>
       </c>
-      <c r="I47" s="48" t="s">
+      <c r="I47" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J47" s="1"/>
@@ -8941,7 +9004,7 @@
       <c r="H48" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="I48" s="48" t="s">
+      <c r="I48" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J48" s="1"/>
@@ -9067,7 +9130,7 @@
       <c r="H49" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="I49" s="48" t="s">
+      <c r="I49" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J49" s="1"/>
@@ -9193,7 +9256,7 @@
       <c r="H50" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="I50" s="48" t="s">
+      <c r="I50" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J50" s="1"/>
@@ -9319,7 +9382,7 @@
       <c r="H51" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="I51" s="48" t="s">
+      <c r="I51" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J51" s="1"/>
@@ -9445,7 +9508,7 @@
       <c r="H52" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="I52" s="48" t="s">
+      <c r="I52" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J52" s="1"/>
@@ -9571,7 +9634,7 @@
       <c r="H53" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="I53" s="48" t="s">
+      <c r="I53" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J53" s="1"/>
@@ -9697,7 +9760,7 @@
       <c r="H54" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="I54" s="48" t="s">
+      <c r="I54" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J54" s="1"/>
@@ -9821,7 +9884,7 @@
         <v>457</v>
       </c>
       <c r="H55" s="1"/>
-      <c r="I55" s="48" t="s">
+      <c r="I55" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J55" s="1"/>
@@ -9945,7 +10008,7 @@
         <v>459</v>
       </c>
       <c r="H56" s="1"/>
-      <c r="I56" s="48" t="s">
+      <c r="I56" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J56" s="1"/>
@@ -10069,7 +10132,7 @@
         <v>461</v>
       </c>
       <c r="H57" s="1"/>
-      <c r="I57" s="48" t="s">
+      <c r="I57" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J57" s="1"/>
@@ -10193,7 +10256,7 @@
         <v>463</v>
       </c>
       <c r="H58" s="1"/>
-      <c r="I58" s="48" t="s">
+      <c r="I58" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J58" s="1"/>
@@ -10319,7 +10382,7 @@
       <c r="H59" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="I59" s="48" t="s">
+      <c r="I59" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J59" s="1"/>
@@ -10445,7 +10508,7 @@
       <c r="H60" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I60" s="48" t="s">
+      <c r="I60" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J60" s="1"/>
@@ -10571,7 +10634,7 @@
       <c r="H61" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="I61" s="48" t="s">
+      <c r="I61" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J61" s="1"/>
@@ -10697,7 +10760,7 @@
       <c r="H62" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="I62" s="48" t="s">
+      <c r="I62" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J62" s="1"/>
@@ -10821,7 +10884,7 @@
         <v>477</v>
       </c>
       <c r="H63" s="1"/>
-      <c r="I63" s="48" t="s">
+      <c r="I63" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J63" s="1"/>
@@ -10945,7 +11008,7 @@
         <v>479</v>
       </c>
       <c r="H64" s="1"/>
-      <c r="I64" s="48" t="s">
+      <c r="I64" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J64" s="1"/>
@@ -11071,7 +11134,7 @@
       <c r="H65" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="I65" s="48" t="s">
+      <c r="I65" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J65" s="1"/>
@@ -11197,7 +11260,7 @@
       <c r="H66" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="I66" s="48" t="s">
+      <c r="I66" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J66" s="1"/>
@@ -11321,7 +11384,7 @@
         <v>487</v>
       </c>
       <c r="H67" s="1"/>
-      <c r="I67" s="48" t="s">
+      <c r="I67" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J67" s="1"/>
@@ -11447,7 +11510,7 @@
         <v>489</v>
       </c>
       <c r="H68" s="1"/>
-      <c r="I68" s="48" t="s">
+      <c r="I68" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J68" s="1"/>
@@ -11575,7 +11638,7 @@
       <c r="H69" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="I69" s="48" t="s">
+      <c r="I69" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J69" s="1"/>
@@ -11703,7 +11766,7 @@
       <c r="H70" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="I70" s="48" t="s">
+      <c r="I70" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J70" s="1"/>
@@ -11831,7 +11894,7 @@
       <c r="H71" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="I71" s="48" t="s">
+      <c r="I71" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J71" s="1"/>
@@ -11959,7 +12022,7 @@
       <c r="H72" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="I72" s="48" t="s">
+      <c r="I72" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J72" s="1"/>
@@ -12087,7 +12150,7 @@
       <c r="H73" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="I73" s="48" t="s">
+      <c r="I73" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J73" s="1"/>
@@ -12215,7 +12278,7 @@
       <c r="H74" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I74" s="48" t="s">
+      <c r="I74" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J74" s="1"/>
@@ -12343,7 +12406,7 @@
       <c r="H75" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="I75" s="48" t="s">
+      <c r="I75" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J75" s="1"/>
@@ -12471,7 +12534,7 @@
       <c r="H76" s="42" t="s">
         <v>511</v>
       </c>
-      <c r="I76" s="48" t="s">
+      <c r="I76" s="51" t="s">
         <v>189</v>
       </c>
       <c r="J76" s="42"/>
@@ -12578,7 +12641,7 @@
       <c r="A77" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="B77" s="32" t="s">
+      <c r="B77" s="42" t="s">
         <v>3</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -12597,7 +12660,9 @@
         <v>562</v>
       </c>
       <c r="H77" s="44"/>
-      <c r="I77" s="44"/>
+      <c r="I77" s="46" t="s">
+        <v>571</v>
+      </c>
       <c r="J77" s="44"/>
       <c r="K77" s="44"/>
       <c r="L77" s="44"/>

</xml_diff>

<commit_message>
Updated changes to run Merge DP test case accordingly
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="584">
   <si>
     <t>Environment</t>
   </si>
@@ -2615,8 +2615,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CV78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AT78" sqref="AT78"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7167,11 +7167,15 @@
       <c r="BD34" s="1"/>
       <c r="BE34" s="1"/>
       <c r="BF34" s="1"/>
-      <c r="BG34" s="1"/>
+      <c r="BG34" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH34" s="1"/>
       <c r="BI34" s="1"/>
       <c r="BJ34" s="1"/>
-      <c r="BK34" s="1"/>
+      <c r="BK34" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL34" s="1"/>
       <c r="BM34" s="1"/>
       <c r="BN34" s="1"/>
@@ -7185,7 +7189,9 @@
       <c r="BV34" s="1"/>
       <c r="BW34" s="1"/>
       <c r="BX34" s="1"/>
-      <c r="BY34" s="1"/>
+      <c r="BY34" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ34" s="1"/>
       <c r="CA34" s="1"/>
       <c r="CB34" s="1"/>
@@ -7297,11 +7303,15 @@
       <c r="BD35" s="1"/>
       <c r="BE35" s="1"/>
       <c r="BF35" s="1"/>
-      <c r="BG35" s="1"/>
+      <c r="BG35" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH35" s="1"/>
       <c r="BI35" s="1"/>
       <c r="BJ35" s="1"/>
-      <c r="BK35" s="1"/>
+      <c r="BK35" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL35" s="1"/>
       <c r="BM35" s="1"/>
       <c r="BN35" s="1"/>
@@ -7315,7 +7325,9 @@
       <c r="BV35" s="1"/>
       <c r="BW35" s="1"/>
       <c r="BX35" s="1"/>
-      <c r="BY35" s="1"/>
+      <c r="BY35" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ35" s="1"/>
       <c r="CA35" s="1"/>
       <c r="CB35" s="1"/>
@@ -7427,11 +7439,15 @@
       <c r="BD36" s="1"/>
       <c r="BE36" s="1"/>
       <c r="BF36" s="1"/>
-      <c r="BG36" s="1"/>
+      <c r="BG36" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH36" s="1"/>
       <c r="BI36" s="1"/>
       <c r="BJ36" s="1"/>
-      <c r="BK36" s="1"/>
+      <c r="BK36" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL36" s="1"/>
       <c r="BM36" s="1"/>
       <c r="BN36" s="1"/>
@@ -7445,7 +7461,9 @@
       <c r="BV36" s="1"/>
       <c r="BW36" s="1"/>
       <c r="BX36" s="1"/>
-      <c r="BY36" s="1"/>
+      <c r="BY36" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ36" s="1"/>
       <c r="CA36" s="1"/>
       <c r="CB36" s="1"/>
@@ -7557,11 +7575,15 @@
       <c r="BD37" s="1"/>
       <c r="BE37" s="1"/>
       <c r="BF37" s="1"/>
-      <c r="BG37" s="1"/>
+      <c r="BG37" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH37" s="1"/>
       <c r="BI37" s="1"/>
       <c r="BJ37" s="1"/>
-      <c r="BK37" s="1"/>
+      <c r="BK37" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL37" s="1"/>
       <c r="BM37" s="1"/>
       <c r="BN37" s="1"/>
@@ -7575,7 +7597,9 @@
       <c r="BV37" s="1"/>
       <c r="BW37" s="1"/>
       <c r="BX37" s="1"/>
-      <c r="BY37" s="1"/>
+      <c r="BY37" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ37" s="1"/>
       <c r="CA37" s="1"/>
       <c r="CB37" s="1"/>
@@ -7687,11 +7711,15 @@
       <c r="BD38" s="1"/>
       <c r="BE38" s="1"/>
       <c r="BF38" s="1"/>
-      <c r="BG38" s="1"/>
+      <c r="BG38" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH38" s="1"/>
       <c r="BI38" s="1"/>
       <c r="BJ38" s="1"/>
-      <c r="BK38" s="1"/>
+      <c r="BK38" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL38" s="1"/>
       <c r="BM38" s="1"/>
       <c r="BN38" s="1"/>
@@ -7705,7 +7733,9 @@
       <c r="BV38" s="1"/>
       <c r="BW38" s="1"/>
       <c r="BX38" s="1"/>
-      <c r="BY38" s="1"/>
+      <c r="BY38" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ38" s="1"/>
       <c r="CA38" s="1"/>
       <c r="CB38" s="1"/>
@@ -7817,11 +7847,15 @@
       <c r="BD39" s="1"/>
       <c r="BE39" s="1"/>
       <c r="BF39" s="1"/>
-      <c r="BG39" s="1"/>
+      <c r="BG39" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH39" s="1"/>
       <c r="BI39" s="1"/>
       <c r="BJ39" s="1"/>
-      <c r="BK39" s="1"/>
+      <c r="BK39" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL39" s="1"/>
       <c r="BM39" s="1"/>
       <c r="BN39" s="1"/>
@@ -7835,7 +7869,9 @@
       <c r="BV39" s="1"/>
       <c r="BW39" s="1"/>
       <c r="BX39" s="1"/>
-      <c r="BY39" s="1"/>
+      <c r="BY39" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ39" s="1"/>
       <c r="CA39" s="1"/>
       <c r="CB39" s="1"/>
@@ -7947,11 +7983,15 @@
       <c r="BD40" s="1"/>
       <c r="BE40" s="1"/>
       <c r="BF40" s="1"/>
-      <c r="BG40" s="1"/>
+      <c r="BG40" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH40" s="1"/>
       <c r="BI40" s="1"/>
       <c r="BJ40" s="1"/>
-      <c r="BK40" s="1"/>
+      <c r="BK40" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL40" s="1"/>
       <c r="BM40" s="1"/>
       <c r="BN40" s="1"/>
@@ -7965,7 +8005,9 @@
       <c r="BV40" s="1"/>
       <c r="BW40" s="1"/>
       <c r="BX40" s="1"/>
-      <c r="BY40" s="1"/>
+      <c r="BY40" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ40" s="1"/>
       <c r="CA40" s="1"/>
       <c r="CB40" s="1"/>
@@ -8077,7 +8119,9 @@
       <c r="BD41" s="1"/>
       <c r="BE41" s="1"/>
       <c r="BF41" s="1"/>
-      <c r="BG41" s="1"/>
+      <c r="BG41" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH41" s="1"/>
       <c r="BI41" s="1"/>
       <c r="BJ41" s="1"/>
@@ -8097,7 +8141,9 @@
       <c r="BV41" s="1"/>
       <c r="BW41" s="1"/>
       <c r="BX41" s="1"/>
-      <c r="BY41" s="1"/>
+      <c r="BY41" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ41" s="1"/>
       <c r="CA41" s="1"/>
       <c r="CB41" s="1"/>
@@ -8215,7 +8261,9 @@
       <c r="BH42" s="1"/>
       <c r="BI42" s="1"/>
       <c r="BJ42" s="1"/>
-      <c r="BK42" s="1"/>
+      <c r="BK42" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL42" s="1"/>
       <c r="BM42" s="1"/>
       <c r="BN42" s="1"/>
@@ -8229,7 +8277,9 @@
       <c r="BV42" s="1"/>
       <c r="BW42" s="1"/>
       <c r="BX42" s="1"/>
-      <c r="BY42" s="1"/>
+      <c r="BY42" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ42" s="1"/>
       <c r="CA42" s="1"/>
       <c r="CB42" s="1"/>
@@ -8341,11 +8391,15 @@
       <c r="BD43" s="1"/>
       <c r="BE43" s="1"/>
       <c r="BF43" s="1"/>
-      <c r="BG43" s="1"/>
+      <c r="BG43" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH43" s="1"/>
       <c r="BI43" s="1"/>
       <c r="BJ43" s="1"/>
-      <c r="BK43" s="1"/>
+      <c r="BK43" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL43" s="1"/>
       <c r="BM43" s="1"/>
       <c r="BN43" s="1"/>
@@ -8473,11 +8527,15 @@
       <c r="BD44" s="1"/>
       <c r="BE44" s="1"/>
       <c r="BF44" s="1"/>
-      <c r="BG44" s="1"/>
+      <c r="BG44" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH44" s="1"/>
       <c r="BI44" s="1"/>
       <c r="BJ44" s="1"/>
-      <c r="BK44" s="1"/>
+      <c r="BK44" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL44" s="1"/>
       <c r="BM44" s="1"/>
       <c r="BN44" s="1"/>
@@ -8491,7 +8549,9 @@
       <c r="BV44" s="1"/>
       <c r="BW44" s="1"/>
       <c r="BX44" s="1"/>
-      <c r="BY44" s="1"/>
+      <c r="BY44" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ44" s="1"/>
       <c r="CA44" s="1"/>
       <c r="CB44" s="1"/>

</xml_diff>

<commit_message>
Merge test  invitation code
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="584">
   <si>
     <t>Environment</t>
   </si>
@@ -2615,8 +2615,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CV78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AS3" sqref="AS3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3071,7 +3071,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -3129,7 +3129,9 @@
       <c r="AP3" s="6"/>
       <c r="AQ3" s="6"/>
       <c r="AR3" s="6"/>
-      <c r="AS3" s="6"/>
+      <c r="AS3" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="AT3" s="6" t="s">
         <v>34</v>
       </c>
@@ -7167,15 +7169,11 @@
       <c r="BD34" s="1"/>
       <c r="BE34" s="1"/>
       <c r="BF34" s="1"/>
-      <c r="BG34" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG34" s="1"/>
       <c r="BH34" s="1"/>
       <c r="BI34" s="1"/>
       <c r="BJ34" s="1"/>
-      <c r="BK34" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK34" s="1"/>
       <c r="BL34" s="1"/>
       <c r="BM34" s="1"/>
       <c r="BN34" s="1"/>
@@ -7189,9 +7187,7 @@
       <c r="BV34" s="1"/>
       <c r="BW34" s="1"/>
       <c r="BX34" s="1"/>
-      <c r="BY34" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY34" s="1"/>
       <c r="BZ34" s="1"/>
       <c r="CA34" s="1"/>
       <c r="CB34" s="1"/>
@@ -7303,15 +7299,11 @@
       <c r="BD35" s="1"/>
       <c r="BE35" s="1"/>
       <c r="BF35" s="1"/>
-      <c r="BG35" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG35" s="1"/>
       <c r="BH35" s="1"/>
       <c r="BI35" s="1"/>
       <c r="BJ35" s="1"/>
-      <c r="BK35" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK35" s="1"/>
       <c r="BL35" s="1"/>
       <c r="BM35" s="1"/>
       <c r="BN35" s="1"/>
@@ -7325,9 +7317,7 @@
       <c r="BV35" s="1"/>
       <c r="BW35" s="1"/>
       <c r="BX35" s="1"/>
-      <c r="BY35" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY35" s="1"/>
       <c r="BZ35" s="1"/>
       <c r="CA35" s="1"/>
       <c r="CB35" s="1"/>
@@ -7439,15 +7429,11 @@
       <c r="BD36" s="1"/>
       <c r="BE36" s="1"/>
       <c r="BF36" s="1"/>
-      <c r="BG36" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG36" s="1"/>
       <c r="BH36" s="1"/>
       <c r="BI36" s="1"/>
       <c r="BJ36" s="1"/>
-      <c r="BK36" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK36" s="1"/>
       <c r="BL36" s="1"/>
       <c r="BM36" s="1"/>
       <c r="BN36" s="1"/>
@@ -7461,9 +7447,7 @@
       <c r="BV36" s="1"/>
       <c r="BW36" s="1"/>
       <c r="BX36" s="1"/>
-      <c r="BY36" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY36" s="1"/>
       <c r="BZ36" s="1"/>
       <c r="CA36" s="1"/>
       <c r="CB36" s="1"/>
@@ -7575,15 +7559,11 @@
       <c r="BD37" s="1"/>
       <c r="BE37" s="1"/>
       <c r="BF37" s="1"/>
-      <c r="BG37" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG37" s="1"/>
       <c r="BH37" s="1"/>
       <c r="BI37" s="1"/>
       <c r="BJ37" s="1"/>
-      <c r="BK37" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK37" s="1"/>
       <c r="BL37" s="1"/>
       <c r="BM37" s="1"/>
       <c r="BN37" s="1"/>
@@ -7597,9 +7577,7 @@
       <c r="BV37" s="1"/>
       <c r="BW37" s="1"/>
       <c r="BX37" s="1"/>
-      <c r="BY37" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY37" s="1"/>
       <c r="BZ37" s="1"/>
       <c r="CA37" s="1"/>
       <c r="CB37" s="1"/>
@@ -7711,15 +7689,11 @@
       <c r="BD38" s="1"/>
       <c r="BE38" s="1"/>
       <c r="BF38" s="1"/>
-      <c r="BG38" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG38" s="1"/>
       <c r="BH38" s="1"/>
       <c r="BI38" s="1"/>
       <c r="BJ38" s="1"/>
-      <c r="BK38" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK38" s="1"/>
       <c r="BL38" s="1"/>
       <c r="BM38" s="1"/>
       <c r="BN38" s="1"/>
@@ -7733,9 +7707,7 @@
       <c r="BV38" s="1"/>
       <c r="BW38" s="1"/>
       <c r="BX38" s="1"/>
-      <c r="BY38" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY38" s="1"/>
       <c r="BZ38" s="1"/>
       <c r="CA38" s="1"/>
       <c r="CB38" s="1"/>
@@ -7847,15 +7819,11 @@
       <c r="BD39" s="1"/>
       <c r="BE39" s="1"/>
       <c r="BF39" s="1"/>
-      <c r="BG39" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG39" s="1"/>
       <c r="BH39" s="1"/>
       <c r="BI39" s="1"/>
       <c r="BJ39" s="1"/>
-      <c r="BK39" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK39" s="1"/>
       <c r="BL39" s="1"/>
       <c r="BM39" s="1"/>
       <c r="BN39" s="1"/>
@@ -7869,9 +7837,7 @@
       <c r="BV39" s="1"/>
       <c r="BW39" s="1"/>
       <c r="BX39" s="1"/>
-      <c r="BY39" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY39" s="1"/>
       <c r="BZ39" s="1"/>
       <c r="CA39" s="1"/>
       <c r="CB39" s="1"/>
@@ -7983,15 +7949,11 @@
       <c r="BD40" s="1"/>
       <c r="BE40" s="1"/>
       <c r="BF40" s="1"/>
-      <c r="BG40" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG40" s="1"/>
       <c r="BH40" s="1"/>
       <c r="BI40" s="1"/>
       <c r="BJ40" s="1"/>
-      <c r="BK40" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK40" s="1"/>
       <c r="BL40" s="1"/>
       <c r="BM40" s="1"/>
       <c r="BN40" s="1"/>
@@ -8005,9 +7967,7 @@
       <c r="BV40" s="1"/>
       <c r="BW40" s="1"/>
       <c r="BX40" s="1"/>
-      <c r="BY40" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY40" s="1"/>
       <c r="BZ40" s="1"/>
       <c r="CA40" s="1"/>
       <c r="CB40" s="1"/>
@@ -8119,9 +8079,7 @@
       <c r="BD41" s="1"/>
       <c r="BE41" s="1"/>
       <c r="BF41" s="1"/>
-      <c r="BG41" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG41" s="1"/>
       <c r="BH41" s="1"/>
       <c r="BI41" s="1"/>
       <c r="BJ41" s="1"/>
@@ -8141,9 +8099,7 @@
       <c r="BV41" s="1"/>
       <c r="BW41" s="1"/>
       <c r="BX41" s="1"/>
-      <c r="BY41" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY41" s="1"/>
       <c r="BZ41" s="1"/>
       <c r="CA41" s="1"/>
       <c r="CB41" s="1"/>
@@ -8261,9 +8217,7 @@
       <c r="BH42" s="1"/>
       <c r="BI42" s="1"/>
       <c r="BJ42" s="1"/>
-      <c r="BK42" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK42" s="1"/>
       <c r="BL42" s="1"/>
       <c r="BM42" s="1"/>
       <c r="BN42" s="1"/>
@@ -8277,9 +8231,7 @@
       <c r="BV42" s="1"/>
       <c r="BW42" s="1"/>
       <c r="BX42" s="1"/>
-      <c r="BY42" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY42" s="1"/>
       <c r="BZ42" s="1"/>
       <c r="CA42" s="1"/>
       <c r="CB42" s="1"/>
@@ -8391,15 +8343,11 @@
       <c r="BD43" s="1"/>
       <c r="BE43" s="1"/>
       <c r="BF43" s="1"/>
-      <c r="BG43" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG43" s="1"/>
       <c r="BH43" s="1"/>
       <c r="BI43" s="1"/>
       <c r="BJ43" s="1"/>
-      <c r="BK43" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK43" s="1"/>
       <c r="BL43" s="1"/>
       <c r="BM43" s="1"/>
       <c r="BN43" s="1"/>
@@ -8527,15 +8475,11 @@
       <c r="BD44" s="1"/>
       <c r="BE44" s="1"/>
       <c r="BF44" s="1"/>
-      <c r="BG44" s="1" t="s">
-        <v>573</v>
-      </c>
+      <c r="BG44" s="1"/>
       <c r="BH44" s="1"/>
       <c r="BI44" s="1"/>
       <c r="BJ44" s="1"/>
-      <c r="BK44" s="1" t="s">
-        <v>572</v>
-      </c>
+      <c r="BK44" s="1"/>
       <c r="BL44" s="1"/>
       <c r="BM44" s="1"/>
       <c r="BN44" s="1"/>
@@ -8549,9 +8493,7 @@
       <c r="BV44" s="1"/>
       <c r="BW44" s="1"/>
       <c r="BX44" s="1"/>
-      <c r="BY44" s="1" t="s">
-        <v>574</v>
-      </c>
+      <c r="BY44" s="1"/>
       <c r="BZ44" s="1"/>
       <c r="CA44" s="1"/>
       <c r="CB44" s="1"/>

</xml_diff>

<commit_message>
Revert "Merge test  invitation code"
This reverts commit eb114890e3eb3502e18dd89966677356664f3951
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="584">
   <si>
     <t>Environment</t>
   </si>
@@ -2615,8 +2615,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CV78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AS3" sqref="AS3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3071,7 +3071,7 @@
         <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -3129,9 +3129,7 @@
       <c r="AP3" s="6"/>
       <c r="AQ3" s="6"/>
       <c r="AR3" s="6"/>
-      <c r="AS3" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="AS3" s="6"/>
       <c r="AT3" s="6" t="s">
         <v>34</v>
       </c>
@@ -7169,11 +7167,15 @@
       <c r="BD34" s="1"/>
       <c r="BE34" s="1"/>
       <c r="BF34" s="1"/>
-      <c r="BG34" s="1"/>
+      <c r="BG34" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH34" s="1"/>
       <c r="BI34" s="1"/>
       <c r="BJ34" s="1"/>
-      <c r="BK34" s="1"/>
+      <c r="BK34" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL34" s="1"/>
       <c r="BM34" s="1"/>
       <c r="BN34" s="1"/>
@@ -7187,7 +7189,9 @@
       <c r="BV34" s="1"/>
       <c r="BW34" s="1"/>
       <c r="BX34" s="1"/>
-      <c r="BY34" s="1"/>
+      <c r="BY34" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ34" s="1"/>
       <c r="CA34" s="1"/>
       <c r="CB34" s="1"/>
@@ -7299,11 +7303,15 @@
       <c r="BD35" s="1"/>
       <c r="BE35" s="1"/>
       <c r="BF35" s="1"/>
-      <c r="BG35" s="1"/>
+      <c r="BG35" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH35" s="1"/>
       <c r="BI35" s="1"/>
       <c r="BJ35" s="1"/>
-      <c r="BK35" s="1"/>
+      <c r="BK35" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL35" s="1"/>
       <c r="BM35" s="1"/>
       <c r="BN35" s="1"/>
@@ -7317,7 +7325,9 @@
       <c r="BV35" s="1"/>
       <c r="BW35" s="1"/>
       <c r="BX35" s="1"/>
-      <c r="BY35" s="1"/>
+      <c r="BY35" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ35" s="1"/>
       <c r="CA35" s="1"/>
       <c r="CB35" s="1"/>
@@ -7429,11 +7439,15 @@
       <c r="BD36" s="1"/>
       <c r="BE36" s="1"/>
       <c r="BF36" s="1"/>
-      <c r="BG36" s="1"/>
+      <c r="BG36" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH36" s="1"/>
       <c r="BI36" s="1"/>
       <c r="BJ36" s="1"/>
-      <c r="BK36" s="1"/>
+      <c r="BK36" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL36" s="1"/>
       <c r="BM36" s="1"/>
       <c r="BN36" s="1"/>
@@ -7447,7 +7461,9 @@
       <c r="BV36" s="1"/>
       <c r="BW36" s="1"/>
       <c r="BX36" s="1"/>
-      <c r="BY36" s="1"/>
+      <c r="BY36" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ36" s="1"/>
       <c r="CA36" s="1"/>
       <c r="CB36" s="1"/>
@@ -7559,11 +7575,15 @@
       <c r="BD37" s="1"/>
       <c r="BE37" s="1"/>
       <c r="BF37" s="1"/>
-      <c r="BG37" s="1"/>
+      <c r="BG37" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH37" s="1"/>
       <c r="BI37" s="1"/>
       <c r="BJ37" s="1"/>
-      <c r="BK37" s="1"/>
+      <c r="BK37" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL37" s="1"/>
       <c r="BM37" s="1"/>
       <c r="BN37" s="1"/>
@@ -7577,7 +7597,9 @@
       <c r="BV37" s="1"/>
       <c r="BW37" s="1"/>
       <c r="BX37" s="1"/>
-      <c r="BY37" s="1"/>
+      <c r="BY37" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ37" s="1"/>
       <c r="CA37" s="1"/>
       <c r="CB37" s="1"/>
@@ -7689,11 +7711,15 @@
       <c r="BD38" s="1"/>
       <c r="BE38" s="1"/>
       <c r="BF38" s="1"/>
-      <c r="BG38" s="1"/>
+      <c r="BG38" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH38" s="1"/>
       <c r="BI38" s="1"/>
       <c r="BJ38" s="1"/>
-      <c r="BK38" s="1"/>
+      <c r="BK38" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL38" s="1"/>
       <c r="BM38" s="1"/>
       <c r="BN38" s="1"/>
@@ -7707,7 +7733,9 @@
       <c r="BV38" s="1"/>
       <c r="BW38" s="1"/>
       <c r="BX38" s="1"/>
-      <c r="BY38" s="1"/>
+      <c r="BY38" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ38" s="1"/>
       <c r="CA38" s="1"/>
       <c r="CB38" s="1"/>
@@ -7819,11 +7847,15 @@
       <c r="BD39" s="1"/>
       <c r="BE39" s="1"/>
       <c r="BF39" s="1"/>
-      <c r="BG39" s="1"/>
+      <c r="BG39" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH39" s="1"/>
       <c r="BI39" s="1"/>
       <c r="BJ39" s="1"/>
-      <c r="BK39" s="1"/>
+      <c r="BK39" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL39" s="1"/>
       <c r="BM39" s="1"/>
       <c r="BN39" s="1"/>
@@ -7837,7 +7869,9 @@
       <c r="BV39" s="1"/>
       <c r="BW39" s="1"/>
       <c r="BX39" s="1"/>
-      <c r="BY39" s="1"/>
+      <c r="BY39" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ39" s="1"/>
       <c r="CA39" s="1"/>
       <c r="CB39" s="1"/>
@@ -7949,11 +7983,15 @@
       <c r="BD40" s="1"/>
       <c r="BE40" s="1"/>
       <c r="BF40" s="1"/>
-      <c r="BG40" s="1"/>
+      <c r="BG40" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH40" s="1"/>
       <c r="BI40" s="1"/>
       <c r="BJ40" s="1"/>
-      <c r="BK40" s="1"/>
+      <c r="BK40" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL40" s="1"/>
       <c r="BM40" s="1"/>
       <c r="BN40" s="1"/>
@@ -7967,7 +8005,9 @@
       <c r="BV40" s="1"/>
       <c r="BW40" s="1"/>
       <c r="BX40" s="1"/>
-      <c r="BY40" s="1"/>
+      <c r="BY40" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ40" s="1"/>
       <c r="CA40" s="1"/>
       <c r="CB40" s="1"/>
@@ -8079,7 +8119,9 @@
       <c r="BD41" s="1"/>
       <c r="BE41" s="1"/>
       <c r="BF41" s="1"/>
-      <c r="BG41" s="1"/>
+      <c r="BG41" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH41" s="1"/>
       <c r="BI41" s="1"/>
       <c r="BJ41" s="1"/>
@@ -8099,7 +8141,9 @@
       <c r="BV41" s="1"/>
       <c r="BW41" s="1"/>
       <c r="BX41" s="1"/>
-      <c r="BY41" s="1"/>
+      <c r="BY41" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ41" s="1"/>
       <c r="CA41" s="1"/>
       <c r="CB41" s="1"/>
@@ -8217,7 +8261,9 @@
       <c r="BH42" s="1"/>
       <c r="BI42" s="1"/>
       <c r="BJ42" s="1"/>
-      <c r="BK42" s="1"/>
+      <c r="BK42" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL42" s="1"/>
       <c r="BM42" s="1"/>
       <c r="BN42" s="1"/>
@@ -8231,7 +8277,9 @@
       <c r="BV42" s="1"/>
       <c r="BW42" s="1"/>
       <c r="BX42" s="1"/>
-      <c r="BY42" s="1"/>
+      <c r="BY42" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ42" s="1"/>
       <c r="CA42" s="1"/>
       <c r="CB42" s="1"/>
@@ -8343,11 +8391,15 @@
       <c r="BD43" s="1"/>
       <c r="BE43" s="1"/>
       <c r="BF43" s="1"/>
-      <c r="BG43" s="1"/>
+      <c r="BG43" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH43" s="1"/>
       <c r="BI43" s="1"/>
       <c r="BJ43" s="1"/>
-      <c r="BK43" s="1"/>
+      <c r="BK43" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL43" s="1"/>
       <c r="BM43" s="1"/>
       <c r="BN43" s="1"/>
@@ -8475,11 +8527,15 @@
       <c r="BD44" s="1"/>
       <c r="BE44" s="1"/>
       <c r="BF44" s="1"/>
-      <c r="BG44" s="1"/>
+      <c r="BG44" s="1" t="s">
+        <v>573</v>
+      </c>
       <c r="BH44" s="1"/>
       <c r="BI44" s="1"/>
       <c r="BJ44" s="1"/>
-      <c r="BK44" s="1"/>
+      <c r="BK44" s="1" t="s">
+        <v>572</v>
+      </c>
       <c r="BL44" s="1"/>
       <c r="BM44" s="1"/>
       <c r="BN44" s="1"/>
@@ -8493,7 +8549,9 @@
       <c r="BV44" s="1"/>
       <c r="BW44" s="1"/>
       <c r="BX44" s="1"/>
-      <c r="BY44" s="1"/>
+      <c r="BY44" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="BZ44" s="1"/>
       <c r="CA44" s="1"/>
       <c r="CB44" s="1"/>

</xml_diff>

<commit_message>
Updated changes for Darr Report
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1511" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="582">
   <si>
     <t>Environment</t>
   </si>
@@ -1904,7 +1904,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="19">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1984,41 +1984,8 @@
       <u val="single"/>
       <color indexed="12"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <u val="single"/>
-      <color indexed="12"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2065,96 +2032,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -2246,7 +2123,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2295,25 +2172,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="11" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="11" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2820,8 +2684,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CV80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3174,7 +3038,7 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="61" t="s">
+      <c r="I2" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J2" s="11"/>
@@ -3294,7 +3158,7 @@
       <c r="H3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="61" t="s">
+      <c r="I3" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J3" s="11"/>
@@ -3492,7 +3356,7 @@
       <c r="H4" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I4" s="61" t="s">
+      <c r="I4" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J4" s="11"/>
@@ -3624,7 +3488,7 @@
       <c r="H5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I5" s="61" t="s">
+      <c r="I5" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J5" s="10"/>
@@ -3756,7 +3620,7 @@
       <c r="H6" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I6" s="61" t="s">
+      <c r="I6" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J6" s="11"/>
@@ -3878,7 +3742,7 @@
       <c r="H7" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I7" s="61" t="s">
+      <c r="I7" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J7" s="10"/>
@@ -4002,7 +3866,7 @@
       <c r="H8" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I8" s="61" t="s">
+      <c r="I8" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J8" s="11"/>
@@ -4126,7 +3990,7 @@
       <c r="H9" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I9" s="61" t="s">
+      <c r="I9" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J9" s="1"/>
@@ -4240,7 +4104,7 @@
         <v>186</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>572</v>
@@ -4258,8 +4122,8 @@
         <v>191</v>
       </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="61" t="s">
-        <v>188</v>
+      <c r="I10" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J10" s="16"/>
       <c r="K10" s="15" t="s">
@@ -4370,7 +4234,7 @@
         <v>187</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>572</v>
@@ -4388,8 +4252,8 @@
         <v>194</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="61" t="s">
-        <v>188</v>
+      <c r="I11" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J11" s="16"/>
       <c r="K11" s="15" t="s">
@@ -4496,7 +4360,7 @@
         <v>196</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>572</v>
@@ -4514,8 +4378,8 @@
         <v>198</v>
       </c>
       <c r="H12" s="15"/>
-      <c r="I12" s="61" t="s">
-        <v>188</v>
+      <c r="I12" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J12" s="16"/>
       <c r="K12" s="15" t="s">
@@ -4622,7 +4486,7 @@
         <v>200</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>572</v>
@@ -4640,8 +4504,8 @@
         <v>202</v>
       </c>
       <c r="H13" s="15"/>
-      <c r="I13" s="61" t="s">
-        <v>188</v>
+      <c r="I13" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J13" s="16"/>
       <c r="K13" s="15" t="s">
@@ -4748,7 +4612,7 @@
         <v>204</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>572</v>
@@ -4766,8 +4630,8 @@
         <v>206</v>
       </c>
       <c r="H14" s="15"/>
-      <c r="I14" s="61" t="s">
-        <v>188</v>
+      <c r="I14" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="15"/>
@@ -4874,7 +4738,7 @@
         <v>207</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>572</v>
@@ -4892,8 +4756,8 @@
         <v>209</v>
       </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="61" t="s">
-        <v>188</v>
+      <c r="I15" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="15" t="s">
@@ -5022,7 +4886,7 @@
         <v>215</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>572</v>
@@ -5040,8 +4904,8 @@
         <v>229</v>
       </c>
       <c r="H16" s="15"/>
-      <c r="I16" s="61" t="s">
-        <v>188</v>
+      <c r="I16" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="15" t="s">
@@ -5182,7 +5046,7 @@
       <c r="H17" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I17" s="61" t="s">
+      <c r="I17" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J17" s="11"/>
@@ -5296,7 +5160,7 @@
         <v>226</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>572</v>
@@ -5312,8 +5176,8 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="61" t="s">
-        <v>188</v>
+      <c r="I18" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="1"/>
@@ -5418,7 +5282,7 @@
         <v>250</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>572</v>
@@ -5434,8 +5298,8 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="61" t="s">
-        <v>188</v>
+      <c r="I19" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="1"/>
@@ -5556,7 +5420,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="61" t="s">
+      <c r="I20" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J20" s="11"/>
@@ -5686,7 +5550,7 @@
       <c r="H21" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I21" s="61" t="s">
+      <c r="I21" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J21" s="1"/>
@@ -5816,7 +5680,7 @@
       <c r="H22" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="I22" s="61" t="s">
+      <c r="I22" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J22" s="1"/>
@@ -5942,7 +5806,7 @@
       <c r="H23" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I23" s="61" t="s">
+      <c r="I23" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J23" s="1"/>
@@ -6074,7 +5938,7 @@
       <c r="H24" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I24" s="61" t="s">
+      <c r="I24" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J24" s="1"/>
@@ -6202,7 +6066,7 @@
       <c r="H25" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="I25" s="61" t="s">
+      <c r="I25" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J25" s="1"/>
@@ -6330,7 +6194,7 @@
       <c r="H26" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="I26" s="61" t="s">
+      <c r="I26" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J26" s="1"/>
@@ -6458,7 +6322,7 @@
       <c r="H27" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="I27" s="61" t="s">
+      <c r="I27" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J27" s="1"/>
@@ -6584,7 +6448,7 @@
       <c r="H28" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="I28" s="61" t="s">
+      <c r="I28" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J28" s="1"/>
@@ -6710,7 +6574,7 @@
       <c r="H29" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="I29" s="61" t="s">
+      <c r="I29" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J29" s="1"/>
@@ -6838,7 +6702,7 @@
       <c r="H30" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="I30" s="61" t="s">
+      <c r="I30" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J30" s="1"/>
@@ -6968,7 +6832,7 @@
       <c r="H31" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="I31" s="61" t="s">
+      <c r="I31" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J31" s="1"/>
@@ -7098,7 +6962,7 @@
       <c r="H32" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I32" s="61" t="s">
+      <c r="I32" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J32" s="1"/>
@@ -7204,7 +7068,7 @@
         <v>502</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>572</v>
@@ -7222,8 +7086,8 @@
         <v>544</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="61" t="s">
-        <v>188</v>
+      <c r="I33" s="46" t="s">
+        <v>574</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -7340,7 +7204,7 @@
         <v>507</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="61" t="s">
+      <c r="I34" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J34" s="1"/>
@@ -7476,7 +7340,7 @@
         <v>516</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="61" t="s">
+      <c r="I35" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J35" s="1"/>
@@ -7612,7 +7476,7 @@
         <v>519</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="61" t="s">
+      <c r="I36" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J36" s="1"/>
@@ -7748,7 +7612,7 @@
         <v>522</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="61" t="s">
+      <c r="I37" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J37" s="1"/>
@@ -7884,7 +7748,7 @@
         <v>525</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="61" t="s">
+      <c r="I38" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J38" s="1"/>
@@ -8020,7 +7884,7 @@
         <v>528</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="61" t="s">
+      <c r="I39" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J39" s="1"/>
@@ -8156,7 +8020,7 @@
         <v>531</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="61" t="s">
+      <c r="I40" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J40" s="1"/>
@@ -8292,7 +8156,7 @@
         <v>534</v>
       </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="61" t="s">
+      <c r="I41" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J41" s="1"/>
@@ -8428,7 +8292,7 @@
         <v>537</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="61" t="s">
+      <c r="I42" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J42" s="1"/>
@@ -8564,7 +8428,7 @@
         <v>540</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="61" t="s">
+      <c r="I43" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J43" s="1"/>
@@ -8700,7 +8564,7 @@
         <v>542</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="61" t="s">
+      <c r="I44" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J44" s="1"/>
@@ -8838,7 +8702,7 @@
       <c r="H45" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I45" s="61" t="s">
+      <c r="I45" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J45" s="1"/>
@@ -8968,7 +8832,7 @@
       <c r="H46" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="I46" s="61" t="s">
+      <c r="I46" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J46" s="1"/>
@@ -9098,7 +8962,7 @@
       <c r="H47" s="21" t="s">
         <v>424</v>
       </c>
-      <c r="I47" s="61" t="s">
+      <c r="I47" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J47" s="1"/>
@@ -9224,7 +9088,7 @@
       <c r="H48" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="I48" s="61" t="s">
+      <c r="I48" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J48" s="1"/>
@@ -9350,7 +9214,7 @@
       <c r="H49" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="I49" s="61" t="s">
+      <c r="I49" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J49" s="1"/>
@@ -9476,7 +9340,7 @@
       <c r="H50" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="I50" s="61" t="s">
+      <c r="I50" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J50" s="1"/>
@@ -9602,7 +9466,7 @@
       <c r="H51" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="I51" s="61" t="s">
+      <c r="I51" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J51" s="1"/>
@@ -9728,7 +9592,7 @@
       <c r="H52" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="I52" s="61" t="s">
+      <c r="I52" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J52" s="1"/>
@@ -9854,7 +9718,7 @@
       <c r="H53" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="I53" s="61" t="s">
+      <c r="I53" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J53" s="1"/>
@@ -9980,7 +9844,7 @@
       <c r="H54" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="I54" s="61" t="s">
+      <c r="I54" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J54" s="1"/>
@@ -10104,7 +9968,7 @@
         <v>447</v>
       </c>
       <c r="H55" s="1"/>
-      <c r="I55" s="61" t="s">
+      <c r="I55" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J55" s="1"/>
@@ -10228,7 +10092,7 @@
         <v>449</v>
       </c>
       <c r="H56" s="1"/>
-      <c r="I56" s="61" t="s">
+      <c r="I56" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J56" s="1"/>
@@ -10352,7 +10216,7 @@
         <v>451</v>
       </c>
       <c r="H57" s="1"/>
-      <c r="I57" s="61" t="s">
+      <c r="I57" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J57" s="1"/>
@@ -10476,7 +10340,7 @@
         <v>453</v>
       </c>
       <c r="H58" s="1"/>
-      <c r="I58" s="61" t="s">
+      <c r="I58" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J58" s="1"/>
@@ -10602,7 +10466,7 @@
       <c r="H59" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="I59" s="61" t="s">
+      <c r="I59" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J59" s="1"/>
@@ -10728,7 +10592,7 @@
       <c r="H60" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="I60" s="61" t="s">
+      <c r="I60" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J60" s="1"/>
@@ -10854,7 +10718,7 @@
       <c r="H61" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="I61" s="61" t="s">
+      <c r="I61" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J61" s="1"/>
@@ -10980,7 +10844,7 @@
       <c r="H62" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="I62" s="61" t="s">
+      <c r="I62" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J62" s="1"/>
@@ -11104,7 +10968,7 @@
         <v>467</v>
       </c>
       <c r="H63" s="1"/>
-      <c r="I63" s="61" t="s">
+      <c r="I63" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J63" s="1"/>
@@ -11228,7 +11092,7 @@
         <v>469</v>
       </c>
       <c r="H64" s="1"/>
-      <c r="I64" s="61" t="s">
+      <c r="I64" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J64" s="1"/>
@@ -11354,7 +11218,7 @@
       <c r="H65" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="I65" s="61" t="s">
+      <c r="I65" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J65" s="1"/>
@@ -11480,7 +11344,7 @@
       <c r="H66" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="I66" s="61" t="s">
+      <c r="I66" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J66" s="1"/>
@@ -11604,7 +11468,7 @@
         <v>477</v>
       </c>
       <c r="H67" s="1"/>
-      <c r="I67" s="61" t="s">
+      <c r="I67" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J67" s="1"/>
@@ -11730,7 +11594,7 @@
         <v>479</v>
       </c>
       <c r="H68" s="1"/>
-      <c r="I68" s="61" t="s">
+      <c r="I68" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J68" s="1"/>
@@ -11858,7 +11722,7 @@
       <c r="H69" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="I69" s="61" t="s">
+      <c r="I69" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J69" s="1"/>
@@ -11986,7 +11850,7 @@
       <c r="H70" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="I70" s="61" t="s">
+      <c r="I70" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J70" s="1"/>
@@ -12114,7 +11978,7 @@
       <c r="H71" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="I71" s="61" t="s">
+      <c r="I71" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J71" s="1"/>
@@ -12242,7 +12106,7 @@
       <c r="H72" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="I72" s="61" t="s">
+      <c r="I72" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J72" s="1"/>
@@ -12370,7 +12234,7 @@
       <c r="H73" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="I73" s="61" t="s">
+      <c r="I73" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J73" s="1"/>
@@ -12498,7 +12362,7 @@
       <c r="H74" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="I74" s="61" t="s">
+      <c r="I74" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J74" s="1"/>
@@ -12626,7 +12490,7 @@
       <c r="H75" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="I75" s="61" t="s">
+      <c r="I75" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J75" s="1"/>
@@ -12754,7 +12618,7 @@
       <c r="H76" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="I76" s="61" t="s">
+      <c r="I76" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J76" s="1"/>
@@ -12880,7 +12744,7 @@
         <v>551</v>
       </c>
       <c r="H77" s="27"/>
-      <c r="I77" s="61" t="s">
+      <c r="I77" s="48" t="s">
         <v>188</v>
       </c>
       <c r="J77" s="27"/>
@@ -13133,8 +12997,8 @@
       <c r="A79" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="B79" s="35" t="s">
-        <v>3</v>
+      <c r="B79" s="36" t="s">
+        <v>11</v>
       </c>
       <c r="C79" s="35" t="s">
         <v>579</v>
@@ -13150,8 +13014,8 @@
       </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-      <c r="I79" s="59" t="s">
-        <v>574</v>
+      <c r="I79" s="48" t="s">
+        <v>188</v>
       </c>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
@@ -13249,8 +13113,8 @@
       <c r="A80" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="B80" s="35" t="s">
-        <v>3</v>
+      <c r="B80" s="36" t="s">
+        <v>11</v>
       </c>
       <c r="C80" s="35" t="s">
         <v>579</v>
@@ -13266,8 +13130,8 @@
       </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-      <c r="I80" s="59" t="s">
-        <v>574</v>
+      <c r="I80" s="48" t="s">
+        <v>188</v>
       </c>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>

</xml_diff>

<commit_message>
Saved report and email report validation added in reports DP.
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3E8F22-1D16-4DDB-96C6-C6751B363B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="582">
   <si>
     <t>Environment</t>
   </si>
@@ -1902,9 +1903,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1974,6 +1975,12 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -1985,7 +1992,7 @@
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2032,6 +2039,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -2123,7 +2135,7 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2135,7 +2147,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="6" applyBorder="1"/>
@@ -2156,7 +2168,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2173,27 +2185,29 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="11" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="11" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4"/>
-    <cellStyle name="Hyperlink 2 2" xfId="11"/>
-    <cellStyle name="Hyperlink 3" xfId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Hyperlink 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="9"/>
-    <cellStyle name="Normal 3" xfId="5"/>
-    <cellStyle name="Normal 3 2" xfId="12"/>
-    <cellStyle name="Normal 4" xfId="3"/>
-    <cellStyle name="Normal 4 2" xfId="10"/>
-    <cellStyle name="Normal 5" xfId="6"/>
-    <cellStyle name="Normal 5 2" xfId="13"/>
-    <cellStyle name="Normal 6" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 4 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 5 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2470,7 +2484,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2512,7 +2526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2554,7 +2568,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -2671,8 +2685,8 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1"/>
-    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2680,12 +2694,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CV80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="CI1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CS10" sqref="CS10:CU13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3038,7 +3052,7 @@
       <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J2" s="11"/>
@@ -3158,7 +3172,7 @@
       <c r="H3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J3" s="11"/>
@@ -3356,7 +3370,7 @@
       <c r="H4" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J4" s="11"/>
@@ -3488,7 +3502,7 @@
       <c r="H5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I5" s="48" t="s">
+      <c r="I5" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J5" s="10"/>
@@ -3620,7 +3634,7 @@
       <c r="H6" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J6" s="11"/>
@@ -3742,7 +3756,7 @@
       <c r="H7" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J7" s="10"/>
@@ -3847,7 +3861,7 @@
       <c r="A8" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -3866,7 +3880,7 @@
       <c r="H8" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J8" s="11"/>
@@ -3971,7 +3985,7 @@
       <c r="A9" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -3990,7 +4004,7 @@
       <c r="H9" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I9" s="48" t="s">
+      <c r="I9" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J9" s="1"/>
@@ -4103,7 +4117,7 @@
       <c r="A10" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -4122,7 +4136,7 @@
         <v>191</v>
       </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="48" t="s">
         <v>574</v>
       </c>
       <c r="J10" s="16"/>
@@ -4144,8 +4158,8 @@
       <c r="T10" s="15"/>
       <c r="U10" s="17"/>
       <c r="V10" s="17"/>
-      <c r="W10" s="18" t="s">
-        <v>341</v>
+      <c r="W10" s="46" t="s">
+        <v>553</v>
       </c>
       <c r="X10" s="17"/>
       <c r="Y10" s="17"/>
@@ -4224,16 +4238,20 @@
       </c>
       <c r="CQ10" s="1"/>
       <c r="CR10" s="1"/>
-      <c r="CS10" s="1"/>
+      <c r="CS10" s="1" t="s">
+        <v>557</v>
+      </c>
       <c r="CT10" s="1"/>
-      <c r="CU10" s="1"/>
+      <c r="CU10" s="47" t="s">
+        <v>558</v>
+      </c>
       <c r="CV10" s="1"/>
     </row>
     <row r="11" spans="1:100">
       <c r="A11" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -4252,7 +4270,7 @@
         <v>194</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="46" t="s">
+      <c r="I11" s="48" t="s">
         <v>574</v>
       </c>
       <c r="J11" s="16"/>
@@ -4270,8 +4288,8 @@
       <c r="T11" s="15"/>
       <c r="U11" s="17"/>
       <c r="V11" s="17"/>
-      <c r="W11" s="18" t="s">
-        <v>341</v>
+      <c r="W11" s="46" t="s">
+        <v>553</v>
       </c>
       <c r="X11" s="17"/>
       <c r="Y11" s="17"/>
@@ -4350,16 +4368,20 @@
       </c>
       <c r="CQ11" s="1"/>
       <c r="CR11" s="1"/>
-      <c r="CS11" s="1"/>
+      <c r="CS11" s="1" t="s">
+        <v>557</v>
+      </c>
       <c r="CT11" s="1"/>
-      <c r="CU11" s="1"/>
+      <c r="CU11" s="47" t="s">
+        <v>558</v>
+      </c>
       <c r="CV11" s="1"/>
     </row>
     <row r="12" spans="1:100">
       <c r="A12" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -4378,7 +4400,7 @@
         <v>198</v>
       </c>
       <c r="H12" s="15"/>
-      <c r="I12" s="46" t="s">
+      <c r="I12" s="48" t="s">
         <v>574</v>
       </c>
       <c r="J12" s="16"/>
@@ -4396,8 +4418,8 @@
       <c r="T12" s="15"/>
       <c r="U12" s="17"/>
       <c r="V12" s="17"/>
-      <c r="W12" s="18" t="s">
-        <v>341</v>
+      <c r="W12" s="46" t="s">
+        <v>553</v>
       </c>
       <c r="X12" s="17"/>
       <c r="Y12" s="17"/>
@@ -4476,16 +4498,20 @@
       </c>
       <c r="CQ12" s="1"/>
       <c r="CR12" s="1"/>
-      <c r="CS12" s="1"/>
+      <c r="CS12" s="1" t="s">
+        <v>557</v>
+      </c>
       <c r="CT12" s="1"/>
-      <c r="CU12" s="1"/>
+      <c r="CU12" s="47" t="s">
+        <v>558</v>
+      </c>
       <c r="CV12" s="1"/>
     </row>
     <row r="13" spans="1:100">
       <c r="A13" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -4504,7 +4530,7 @@
         <v>202</v>
       </c>
       <c r="H13" s="15"/>
-      <c r="I13" s="46" t="s">
+      <c r="I13" s="48" t="s">
         <v>574</v>
       </c>
       <c r="J13" s="16"/>
@@ -4522,8 +4548,8 @@
       <c r="T13" s="15"/>
       <c r="U13" s="17"/>
       <c r="V13" s="17"/>
-      <c r="W13" s="18" t="s">
-        <v>341</v>
+      <c r="W13" s="46" t="s">
+        <v>553</v>
       </c>
       <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
@@ -4602,17 +4628,21 @@
       </c>
       <c r="CQ13" s="1"/>
       <c r="CR13" s="1"/>
-      <c r="CS13" s="1"/>
+      <c r="CS13" s="1" t="s">
+        <v>557</v>
+      </c>
       <c r="CT13" s="1"/>
-      <c r="CU13" s="1"/>
+      <c r="CU13" s="47" t="s">
+        <v>558</v>
+      </c>
       <c r="CV13" s="1"/>
     </row>
     <row r="14" spans="1:100">
       <c r="A14" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B14" s="36" t="s">
-        <v>3</v>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>572</v>
@@ -4630,8 +4660,8 @@
         <v>206</v>
       </c>
       <c r="H14" s="15"/>
-      <c r="I14" s="46" t="s">
-        <v>574</v>
+      <c r="I14" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="J14" s="16"/>
       <c r="K14" s="15"/>
@@ -4737,8 +4767,8 @@
       <c r="A15" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="B15" s="36" t="s">
-        <v>3</v>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>572</v>
@@ -4756,8 +4786,8 @@
         <v>209</v>
       </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="46" t="s">
-        <v>574</v>
+      <c r="I15" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="J15" s="16"/>
       <c r="K15" s="15" t="s">
@@ -4885,8 +4915,8 @@
       <c r="A16" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="B16" s="36" t="s">
-        <v>3</v>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>572</v>
@@ -4904,8 +4934,8 @@
         <v>229</v>
       </c>
       <c r="H16" s="15"/>
-      <c r="I16" s="46" t="s">
-        <v>574</v>
+      <c r="I16" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="15" t="s">
@@ -5027,7 +5057,7 @@
       <c r="A17" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -5046,7 +5076,7 @@
       <c r="H17" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="I17" s="48" t="s">
+      <c r="I17" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J17" s="11"/>
@@ -5159,8 +5189,8 @@
       <c r="A18" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>3</v>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>572</v>
@@ -5176,8 +5206,8 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="46" t="s">
-        <v>574</v>
+      <c r="I18" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="1"/>
@@ -5281,8 +5311,8 @@
       <c r="A19" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>3</v>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>572</v>
@@ -5298,8 +5328,8 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="46" t="s">
-        <v>574</v>
+      <c r="I19" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="1"/>
@@ -5403,7 +5433,7 @@
       <c r="A20" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -5420,7 +5450,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="48" t="s">
+      <c r="I20" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J20" s="11"/>
@@ -5529,7 +5559,7 @@
       <c r="A21" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -5550,7 +5580,7 @@
       <c r="H21" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I21" s="48" t="s">
+      <c r="I21" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J21" s="1"/>
@@ -5659,7 +5689,7 @@
       <c r="A22" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -5680,7 +5710,7 @@
       <c r="H22" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="I22" s="48" t="s">
+      <c r="I22" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J22" s="1"/>
@@ -5785,7 +5815,7 @@
       <c r="A23" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -5806,7 +5836,7 @@
       <c r="H23" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I23" s="48" t="s">
+      <c r="I23" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J23" s="1"/>
@@ -5917,7 +5947,7 @@
       <c r="A24" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -5938,7 +5968,7 @@
       <c r="H24" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I24" s="48" t="s">
+      <c r="I24" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J24" s="1"/>
@@ -6045,7 +6075,7 @@
       <c r="A25" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -6066,7 +6096,7 @@
       <c r="H25" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="I25" s="48" t="s">
+      <c r="I25" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J25" s="1"/>
@@ -6173,7 +6203,7 @@
       <c r="A26" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -6194,7 +6224,7 @@
       <c r="H26" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="I26" s="48" t="s">
+      <c r="I26" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J26" s="1"/>
@@ -6301,7 +6331,7 @@
       <c r="A27" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -6322,7 +6352,7 @@
       <c r="H27" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="I27" s="48" t="s">
+      <c r="I27" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J27" s="1"/>
@@ -6448,7 +6478,7 @@
       <c r="H28" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="I28" s="48" t="s">
+      <c r="I28" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J28" s="1"/>
@@ -6574,7 +6604,7 @@
       <c r="H29" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="I29" s="48" t="s">
+      <c r="I29" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J29" s="1"/>
@@ -6702,7 +6732,7 @@
       <c r="H30" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="I30" s="48" t="s">
+      <c r="I30" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J30" s="1"/>
@@ -6832,7 +6862,7 @@
       <c r="H31" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="I31" s="48" t="s">
+      <c r="I31" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J31" s="1"/>
@@ -6962,7 +6992,7 @@
       <c r="H32" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="I32" s="48" t="s">
+      <c r="I32" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J32" s="1"/>
@@ -7068,7 +7098,7 @@
         <v>502</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>572</v>
@@ -7086,8 +7116,8 @@
         <v>544</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="46" t="s">
-        <v>574</v>
+      <c r="I33" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -7204,7 +7234,7 @@
         <v>507</v>
       </c>
       <c r="H34" s="1"/>
-      <c r="I34" s="48" t="s">
+      <c r="I34" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J34" s="1"/>
@@ -7340,7 +7370,7 @@
         <v>516</v>
       </c>
       <c r="H35" s="1"/>
-      <c r="I35" s="48" t="s">
+      <c r="I35" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J35" s="1"/>
@@ -7476,7 +7506,7 @@
         <v>519</v>
       </c>
       <c r="H36" s="1"/>
-      <c r="I36" s="48" t="s">
+      <c r="I36" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J36" s="1"/>
@@ -7612,7 +7642,7 @@
         <v>522</v>
       </c>
       <c r="H37" s="1"/>
-      <c r="I37" s="48" t="s">
+      <c r="I37" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J37" s="1"/>
@@ -7748,7 +7778,7 @@
         <v>525</v>
       </c>
       <c r="H38" s="1"/>
-      <c r="I38" s="48" t="s">
+      <c r="I38" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J38" s="1"/>
@@ -7884,7 +7914,7 @@
         <v>528</v>
       </c>
       <c r="H39" s="1"/>
-      <c r="I39" s="48" t="s">
+      <c r="I39" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J39" s="1"/>
@@ -8020,7 +8050,7 @@
         <v>531</v>
       </c>
       <c r="H40" s="1"/>
-      <c r="I40" s="48" t="s">
+      <c r="I40" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J40" s="1"/>
@@ -8156,7 +8186,7 @@
         <v>534</v>
       </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="48" t="s">
+      <c r="I41" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J41" s="1"/>
@@ -8292,7 +8322,7 @@
         <v>537</v>
       </c>
       <c r="H42" s="1"/>
-      <c r="I42" s="48" t="s">
+      <c r="I42" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J42" s="1"/>
@@ -8428,7 +8458,7 @@
         <v>540</v>
       </c>
       <c r="H43" s="1"/>
-      <c r="I43" s="48" t="s">
+      <c r="I43" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J43" s="1"/>
@@ -8564,7 +8594,7 @@
         <v>542</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="48" t="s">
+      <c r="I44" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J44" s="1"/>
@@ -8702,7 +8732,7 @@
       <c r="H45" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I45" s="48" t="s">
+      <c r="I45" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J45" s="1"/>
@@ -8832,7 +8862,7 @@
       <c r="H46" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="I46" s="48" t="s">
+      <c r="I46" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J46" s="1"/>
@@ -8962,7 +8992,7 @@
       <c r="H47" s="21" t="s">
         <v>424</v>
       </c>
-      <c r="I47" s="48" t="s">
+      <c r="I47" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J47" s="1"/>
@@ -9088,7 +9118,7 @@
       <c r="H48" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="I48" s="48" t="s">
+      <c r="I48" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J48" s="1"/>
@@ -9214,7 +9244,7 @@
       <c r="H49" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="I49" s="48" t="s">
+      <c r="I49" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J49" s="1"/>
@@ -9340,7 +9370,7 @@
       <c r="H50" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="I50" s="48" t="s">
+      <c r="I50" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J50" s="1"/>
@@ -9466,7 +9496,7 @@
       <c r="H51" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="I51" s="48" t="s">
+      <c r="I51" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J51" s="1"/>
@@ -9592,7 +9622,7 @@
       <c r="H52" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="I52" s="48" t="s">
+      <c r="I52" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J52" s="1"/>
@@ -9718,7 +9748,7 @@
       <c r="H53" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="I53" s="48" t="s">
+      <c r="I53" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J53" s="1"/>
@@ -9844,7 +9874,7 @@
       <c r="H54" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="I54" s="48" t="s">
+      <c r="I54" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J54" s="1"/>
@@ -9968,7 +9998,7 @@
         <v>447</v>
       </c>
       <c r="H55" s="1"/>
-      <c r="I55" s="48" t="s">
+      <c r="I55" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J55" s="1"/>
@@ -10092,7 +10122,7 @@
         <v>449</v>
       </c>
       <c r="H56" s="1"/>
-      <c r="I56" s="48" t="s">
+      <c r="I56" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J56" s="1"/>
@@ -10216,7 +10246,7 @@
         <v>451</v>
       </c>
       <c r="H57" s="1"/>
-      <c r="I57" s="48" t="s">
+      <c r="I57" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J57" s="1"/>
@@ -10340,7 +10370,7 @@
         <v>453</v>
       </c>
       <c r="H58" s="1"/>
-      <c r="I58" s="48" t="s">
+      <c r="I58" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J58" s="1"/>
@@ -10466,7 +10496,7 @@
       <c r="H59" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="I59" s="48" t="s">
+      <c r="I59" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J59" s="1"/>
@@ -10592,7 +10622,7 @@
       <c r="H60" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="I60" s="48" t="s">
+      <c r="I60" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J60" s="1"/>
@@ -10718,7 +10748,7 @@
       <c r="H61" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="I61" s="48" t="s">
+      <c r="I61" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J61" s="1"/>
@@ -10844,7 +10874,7 @@
       <c r="H62" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="I62" s="48" t="s">
+      <c r="I62" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J62" s="1"/>
@@ -10968,7 +10998,7 @@
         <v>467</v>
       </c>
       <c r="H63" s="1"/>
-      <c r="I63" s="48" t="s">
+      <c r="I63" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J63" s="1"/>
@@ -11092,7 +11122,7 @@
         <v>469</v>
       </c>
       <c r="H64" s="1"/>
-      <c r="I64" s="48" t="s">
+      <c r="I64" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J64" s="1"/>
@@ -11218,7 +11248,7 @@
       <c r="H65" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="I65" s="48" t="s">
+      <c r="I65" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J65" s="1"/>
@@ -11344,7 +11374,7 @@
       <c r="H66" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="I66" s="48" t="s">
+      <c r="I66" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J66" s="1"/>
@@ -11468,7 +11498,7 @@
         <v>477</v>
       </c>
       <c r="H67" s="1"/>
-      <c r="I67" s="48" t="s">
+      <c r="I67" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J67" s="1"/>
@@ -11594,7 +11624,7 @@
         <v>479</v>
       </c>
       <c r="H68" s="1"/>
-      <c r="I68" s="48" t="s">
+      <c r="I68" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J68" s="1"/>
@@ -11722,7 +11752,7 @@
       <c r="H69" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="I69" s="48" t="s">
+      <c r="I69" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J69" s="1"/>
@@ -11850,7 +11880,7 @@
       <c r="H70" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="I70" s="48" t="s">
+      <c r="I70" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J70" s="1"/>
@@ -11978,7 +12008,7 @@
       <c r="H71" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="I71" s="48" t="s">
+      <c r="I71" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J71" s="1"/>
@@ -12106,7 +12136,7 @@
       <c r="H72" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="I72" s="48" t="s">
+      <c r="I72" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J72" s="1"/>
@@ -12234,7 +12264,7 @@
       <c r="H73" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="I73" s="48" t="s">
+      <c r="I73" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J73" s="1"/>
@@ -12362,7 +12392,7 @@
       <c r="H74" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="I74" s="48" t="s">
+      <c r="I74" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J74" s="1"/>
@@ -12490,7 +12520,7 @@
       <c r="H75" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="I75" s="48" t="s">
+      <c r="I75" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J75" s="1"/>
@@ -12618,7 +12648,7 @@
       <c r="H76" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="I76" s="48" t="s">
+      <c r="I76" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J76" s="1"/>
@@ -12744,7 +12774,7 @@
         <v>551</v>
       </c>
       <c r="H77" s="27"/>
-      <c r="I77" s="48" t="s">
+      <c r="I77" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J77" s="27"/>
@@ -12861,7 +12891,7 @@
       <c r="A78" s="36" t="s">
         <v>563</v>
       </c>
-      <c r="B78" s="36" t="s">
+      <c r="B78" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C78" s="36" t="s">
@@ -12997,7 +13027,7 @@
       <c r="A79" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="B79" s="36" t="s">
+      <c r="B79" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C79" s="35" t="s">
@@ -13014,7 +13044,7 @@
       </c>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-      <c r="I79" s="48" t="s">
+      <c r="I79" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J79" s="1"/>
@@ -13113,7 +13143,7 @@
       <c r="A80" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="B80" s="36" t="s">
+      <c r="B80" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C80" s="35" t="s">
@@ -13130,7 +13160,7 @@
       </c>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-      <c r="I80" s="48" t="s">
+      <c r="I80" s="50" t="s">
         <v>188</v>
       </c>
       <c r="J80" s="1"/>
@@ -13228,12 +13258,19 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com"/>
-    <hyperlink ref="W10" r:id="rId2"/>
-    <hyperlink ref="W11:W16" r:id="rId3" display="amulla@zarca.com,vgrandhi@zarca.com"/>
-    <hyperlink ref="W14" r:id="rId4"/>
+    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="W11:W16" r:id="rId2" display="amulla@zarca.com,vgrandhi@zarca.com" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="W14" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="W10" r:id="rId4" display="ayadav@zarca.com" xr:uid="{7E315314-162D-48D2-A54E-BDA672EE5F35}"/>
+    <hyperlink ref="W11" r:id="rId5" display="ayadav@zarca.com" xr:uid="{AC56E8BF-CE80-486D-BACA-E21CCB75B917}"/>
+    <hyperlink ref="W12" r:id="rId6" display="ayadav@zarca.com" xr:uid="{2272B8D0-F69B-4F19-9CD3-9D7D1478CEB2}"/>
+    <hyperlink ref="W13" r:id="rId7" display="ayadav@zarca.com" xr:uid="{15258BD1-E46B-4AA1-8C46-49A5AB57F971}"/>
+    <hyperlink ref="CU10" r:id="rId8" xr:uid="{CB2D456C-6B6D-4B78-8FCE-7F365AE87228}"/>
+    <hyperlink ref="CU11" r:id="rId9" xr:uid="{52EC5122-497E-44F3-AC5E-394905BB2BCC}"/>
+    <hyperlink ref="CU12" r:id="rId10" xr:uid="{3D7E0F51-C5D3-4868-A8E8-06210C686C08}"/>
+    <hyperlink ref="CU13" r:id="rId11" xr:uid="{13AF6389-2348-4972-B647-1E24F2576CB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Multi Question Branching data validation
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDB3D49-7AE3-4AC5-98B2-08013A5732C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="660">
   <si>
     <t>Environment</t>
   </si>
@@ -2118,11 +2117,26 @@
   <si>
     <t>account_id</t>
   </si>
+  <si>
+    <t>SID: 1382, mqb</t>
+  </si>
+  <si>
+    <t>Multi Question Branching data testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page </t>
+  </si>
+  <si>
+    <t>Qtitle, AnswerOptions, Page no validation</t>
+  </si>
+  <si>
+    <t>Smoke_TC109</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -2378,19 +2392,19 @@
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Hyperlink 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Hyperlink 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="4"/>
+    <cellStyle name="Hyperlink 2 2" xfId="11"/>
+    <cellStyle name="Hyperlink 3" xfId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 4 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 5 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="9"/>
+    <cellStyle name="Normal 3" xfId="5"/>
+    <cellStyle name="Normal 3 2" xfId="12"/>
+    <cellStyle name="Normal 4" xfId="3"/>
+    <cellStyle name="Normal 4 2" xfId="10"/>
+    <cellStyle name="Normal 5" xfId="6"/>
+    <cellStyle name="Normal 5 2" xfId="13"/>
+    <cellStyle name="Normal 6" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2667,7 +2681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2709,7 +2723,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2751,7 +2765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -2868,8 +2882,8 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -2877,12 +2891,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CW104"/>
+  <dimension ref="A1:CW105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="CR8" sqref="CR8"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16472,20 +16486,145 @@
         <v>178</v>
       </c>
     </row>
+    <row r="105" spans="1:101">
+      <c r="A105" s="48" t="s">
+        <v>659</v>
+      </c>
+      <c r="B105" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" s="48" t="s">
+        <v>579</v>
+      </c>
+      <c r="D105" s="48" t="s">
+        <v>573</v>
+      </c>
+      <c r="E105" s="48" t="s">
+        <v>565</v>
+      </c>
+      <c r="F105" s="48" t="s">
+        <v>656</v>
+      </c>
+      <c r="G105" s="27" t="s">
+        <v>658</v>
+      </c>
+      <c r="H105" s="1"/>
+      <c r="I105" s="50"/>
+      <c r="J105" s="1"/>
+      <c r="K105" s="1"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="31" t="s">
+        <v>657</v>
+      </c>
+      <c r="P105" s="31"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="1"/>
+      <c r="S105" s="1"/>
+      <c r="T105" s="1"/>
+      <c r="U105" s="1"/>
+      <c r="V105" s="1"/>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+      <c r="Y105" s="1"/>
+      <c r="Z105" s="1"/>
+      <c r="AA105" s="1"/>
+      <c r="AB105" s="1"/>
+      <c r="AC105" s="1"/>
+      <c r="AD105" s="1"/>
+      <c r="AE105" s="1"/>
+      <c r="AF105" s="1"/>
+      <c r="AG105" s="1"/>
+      <c r="AH105" s="1"/>
+      <c r="AI105" s="1"/>
+      <c r="AJ105" s="1"/>
+      <c r="AK105" s="1"/>
+      <c r="AL105" s="1"/>
+      <c r="AM105" s="1"/>
+      <c r="AN105" s="1"/>
+      <c r="AO105" s="1"/>
+      <c r="AP105" s="1"/>
+      <c r="AQ105" s="1"/>
+      <c r="AR105" s="1"/>
+      <c r="AS105" s="1"/>
+      <c r="AT105" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="AU105" s="1"/>
+      <c r="AV105" s="1"/>
+      <c r="AW105" s="24"/>
+      <c r="AX105" s="1"/>
+      <c r="AY105" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ105" s="1"/>
+      <c r="BA105" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="BB105" s="1"/>
+      <c r="BC105" s="1"/>
+      <c r="BD105" s="27"/>
+      <c r="BE105" s="27"/>
+      <c r="BF105" s="27"/>
+      <c r="BG105" s="27"/>
+      <c r="BH105" s="27"/>
+      <c r="BI105" s="27"/>
+      <c r="BJ105" s="27"/>
+      <c r="BK105" s="27"/>
+      <c r="BL105" s="27"/>
+      <c r="BM105" s="27"/>
+      <c r="BN105" s="27"/>
+      <c r="BO105" s="27"/>
+      <c r="BP105" s="27"/>
+      <c r="BQ105" s="27"/>
+      <c r="BR105" s="27"/>
+      <c r="BS105" s="27"/>
+      <c r="BT105" s="27"/>
+      <c r="BU105" s="27"/>
+      <c r="BV105" s="27"/>
+      <c r="BW105" s="27"/>
+      <c r="BX105" s="27"/>
+      <c r="BY105" s="27"/>
+      <c r="BZ105" s="27"/>
+      <c r="CA105" s="27"/>
+      <c r="CB105" s="27"/>
+      <c r="CC105" s="27"/>
+      <c r="CD105" s="27"/>
+      <c r="CE105" s="27"/>
+      <c r="CF105" s="27"/>
+      <c r="CG105" s="27"/>
+      <c r="CH105" s="27"/>
+      <c r="CI105" s="28"/>
+      <c r="CJ105" s="27"/>
+      <c r="CK105" s="27"/>
+      <c r="CL105" s="27"/>
+      <c r="CM105" s="27"/>
+      <c r="CN105" s="27"/>
+      <c r="CO105" s="27"/>
+      <c r="CP105" s="27"/>
+      <c r="CQ105" s="1"/>
+      <c r="CR105" s="27"/>
+      <c r="CS105" s="25"/>
+      <c r="CT105" s="51"/>
+      <c r="CU105" s="23"/>
+      <c r="CV105" s="1"/>
+      <c r="CW105" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="W11:W16" r:id="rId2" display="amulla@zarca.com,vgrandhi@zarca.com" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="W14" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="W10" r:id="rId4" display="ayadav@zarca.com" xr:uid="{7E315314-162D-48D2-A54E-BDA672EE5F35}"/>
-    <hyperlink ref="W11" r:id="rId5" display="ayadav@zarca.com" xr:uid="{AC56E8BF-CE80-486D-BACA-E21CCB75B917}"/>
-    <hyperlink ref="W12" r:id="rId6" display="ayadav@zarca.com" xr:uid="{2272B8D0-F69B-4F19-9CD3-9D7D1478CEB2}"/>
-    <hyperlink ref="W13" r:id="rId7" display="ayadav@zarca.com" xr:uid="{15258BD1-E46B-4AA1-8C46-49A5AB57F971}"/>
-    <hyperlink ref="CU10" r:id="rId8" xr:uid="{CB2D456C-6B6D-4B78-8FCE-7F365AE87228}"/>
-    <hyperlink ref="CU11" r:id="rId9" xr:uid="{52EC5122-497E-44F3-AC5E-394905BB2BCC}"/>
-    <hyperlink ref="CU12" r:id="rId10" xr:uid="{3D7E0F51-C5D3-4868-A8E8-06210C686C08}"/>
-    <hyperlink ref="CU13" r:id="rId11" xr:uid="{13AF6389-2348-4972-B647-1E24F2576CB1}"/>
+    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com"/>
+    <hyperlink ref="W11:W16" r:id="rId2" display="amulla@zarca.com,vgrandhi@zarca.com"/>
+    <hyperlink ref="W14" r:id="rId3"/>
+    <hyperlink ref="W10" r:id="rId4" display="ayadav@zarca.com"/>
+    <hyperlink ref="W11" r:id="rId5" display="ayadav@zarca.com"/>
+    <hyperlink ref="W12" r:id="rId6" display="ayadav@zarca.com"/>
+    <hyperlink ref="W13" r:id="rId7" display="ayadav@zarca.com"/>
+    <hyperlink ref="CU10" r:id="rId8"/>
+    <hyperlink ref="CU11" r:id="rId9"/>
+    <hyperlink ref="CU12" r:id="rId10"/>
+    <hyperlink ref="CU13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>

</xml_diff>

<commit_message>
Changes made in excel files only
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48075ED-F5A2-402B-A975-29B46B3699E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -2506,7 +2505,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -2764,19 +2763,19 @@
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Hyperlink 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Hyperlink 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="4"/>
+    <cellStyle name="Hyperlink 2 2" xfId="11"/>
+    <cellStyle name="Hyperlink 3" xfId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 4 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 5 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="9"/>
+    <cellStyle name="Normal 3" xfId="5"/>
+    <cellStyle name="Normal 3 2" xfId="12"/>
+    <cellStyle name="Normal 4" xfId="3"/>
+    <cellStyle name="Normal 4 2" xfId="10"/>
+    <cellStyle name="Normal 5" xfId="6"/>
+    <cellStyle name="Normal 5 2" xfId="13"/>
+    <cellStyle name="Normal 6" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3053,7 +3052,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3095,7 +3094,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3137,7 +3136,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -3254,8 +3253,8 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -3263,12 +3262,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CZ148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4869,7 +4868,7 @@
         <v>187</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>572</v>
@@ -5003,7 +5002,7 @@
         <v>196</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>572</v>
@@ -5137,7 +5136,7 @@
         <v>200</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>572</v>
@@ -14156,8 +14155,8 @@
       <c r="A81" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="B81" s="48" t="s">
-        <v>3</v>
+      <c r="B81" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C81" s="48" t="s">
         <v>579</v>
@@ -14282,8 +14281,8 @@
       <c r="A82" s="48" t="s">
         <v>586</v>
       </c>
-      <c r="B82" s="48" t="s">
-        <v>3</v>
+      <c r="B82" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C82" s="48" t="s">
         <v>579</v>
@@ -14408,8 +14407,8 @@
       <c r="A83" s="48" t="s">
         <v>589</v>
       </c>
-      <c r="B83" s="48" t="s">
-        <v>3</v>
+      <c r="B83" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C83" s="48" t="s">
         <v>579</v>
@@ -14534,8 +14533,8 @@
       <c r="A84" s="48" t="s">
         <v>592</v>
       </c>
-      <c r="B84" s="48" t="s">
-        <v>3</v>
+      <c r="B84" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C84" s="48" t="s">
         <v>579</v>
@@ -14660,8 +14659,8 @@
       <c r="A85" s="48" t="s">
         <v>595</v>
       </c>
-      <c r="B85" s="48" t="s">
-        <v>3</v>
+      <c r="B85" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C85" s="48" t="s">
         <v>579</v>
@@ -14786,8 +14785,8 @@
       <c r="A86" s="48" t="s">
         <v>598</v>
       </c>
-      <c r="B86" s="48" t="s">
-        <v>3</v>
+      <c r="B86" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C86" s="48" t="s">
         <v>579</v>
@@ -14912,8 +14911,8 @@
       <c r="A87" s="48" t="s">
         <v>601</v>
       </c>
-      <c r="B87" s="48" t="s">
-        <v>3</v>
+      <c r="B87" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C87" s="48" t="s">
         <v>579</v>
@@ -15038,8 +15037,8 @@
       <c r="A88" s="48" t="s">
         <v>604</v>
       </c>
-      <c r="B88" s="48" t="s">
-        <v>3</v>
+      <c r="B88" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C88" s="48" t="s">
         <v>579</v>
@@ -15164,8 +15163,8 @@
       <c r="A89" s="48" t="s">
         <v>606</v>
       </c>
-      <c r="B89" s="48" t="s">
-        <v>3</v>
+      <c r="B89" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C89" s="48" t="s">
         <v>579</v>
@@ -15290,8 +15289,8 @@
       <c r="A90" s="48" t="s">
         <v>609</v>
       </c>
-      <c r="B90" s="48" t="s">
-        <v>3</v>
+      <c r="B90" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C90" s="48" t="s">
         <v>579</v>
@@ -15416,7 +15415,7 @@
       <c r="A91" s="48" t="s">
         <v>612</v>
       </c>
-      <c r="B91" s="48" t="s">
+      <c r="B91" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C91" s="48" t="s">
@@ -15542,8 +15541,8 @@
       <c r="A92" s="48" t="s">
         <v>615</v>
       </c>
-      <c r="B92" s="48" t="s">
-        <v>3</v>
+      <c r="B92" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C92" s="48" t="s">
         <v>579</v>
@@ -15668,8 +15667,8 @@
       <c r="A93" s="48" t="s">
         <v>618</v>
       </c>
-      <c r="B93" s="48" t="s">
-        <v>3</v>
+      <c r="B93" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C93" s="48" t="s">
         <v>579</v>
@@ -15794,8 +15793,8 @@
       <c r="A94" s="48" t="s">
         <v>621</v>
       </c>
-      <c r="B94" s="48" t="s">
-        <v>3</v>
+      <c r="B94" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C94" s="48" t="s">
         <v>579</v>
@@ -15920,8 +15919,8 @@
       <c r="A95" s="48" t="s">
         <v>624</v>
       </c>
-      <c r="B95" s="48" t="s">
-        <v>3</v>
+      <c r="B95" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C95" s="48" t="s">
         <v>579</v>
@@ -16046,8 +16045,8 @@
       <c r="A96" s="48" t="s">
         <v>627</v>
       </c>
-      <c r="B96" s="48" t="s">
-        <v>3</v>
+      <c r="B96" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C96" s="48" t="s">
         <v>579</v>
@@ -16172,8 +16171,8 @@
       <c r="A97" s="48" t="s">
         <v>630</v>
       </c>
-      <c r="B97" s="48" t="s">
-        <v>3</v>
+      <c r="B97" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C97" s="48" t="s">
         <v>579</v>
@@ -16298,8 +16297,8 @@
       <c r="A98" s="48" t="s">
         <v>633</v>
       </c>
-      <c r="B98" s="48" t="s">
-        <v>3</v>
+      <c r="B98" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C98" s="48" t="s">
         <v>579</v>
@@ -16424,8 +16423,8 @@
       <c r="A99" s="48" t="s">
         <v>636</v>
       </c>
-      <c r="B99" s="48" t="s">
-        <v>3</v>
+      <c r="B99" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C99" s="48" t="s">
         <v>579</v>
@@ -16550,8 +16549,8 @@
       <c r="A100" s="48" t="s">
         <v>639</v>
       </c>
-      <c r="B100" s="48" t="s">
-        <v>3</v>
+      <c r="B100" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C100" s="48" t="s">
         <v>579</v>
@@ -16676,8 +16675,8 @@
       <c r="A101" s="48" t="s">
         <v>642</v>
       </c>
-      <c r="B101" s="48" t="s">
-        <v>3</v>
+      <c r="B101" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C101" s="48" t="s">
         <v>579</v>
@@ -16802,8 +16801,8 @@
       <c r="A102" s="48" t="s">
         <v>645</v>
       </c>
-      <c r="B102" s="48" t="s">
-        <v>3</v>
+      <c r="B102" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C102" s="48" t="s">
         <v>579</v>
@@ -16928,8 +16927,8 @@
       <c r="A103" s="48" t="s">
         <v>648</v>
       </c>
-      <c r="B103" s="48" t="s">
-        <v>3</v>
+      <c r="B103" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C103" s="48" t="s">
         <v>579</v>
@@ -17054,8 +17053,8 @@
       <c r="A104" s="48" t="s">
         <v>651</v>
       </c>
-      <c r="B104" s="48" t="s">
-        <v>3</v>
+      <c r="B104" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C104" s="48" t="s">
         <v>579</v>
@@ -17180,8 +17179,8 @@
       <c r="A105" s="48" t="s">
         <v>659</v>
       </c>
-      <c r="B105" s="48" t="s">
-        <v>3</v>
+      <c r="B105" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C105" s="48" t="s">
         <v>579</v>
@@ -17308,8 +17307,8 @@
       <c r="A106" s="49" t="s">
         <v>660</v>
       </c>
-      <c r="B106" s="48" t="s">
-        <v>3</v>
+      <c r="B106" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C106" s="49" t="s">
         <v>579</v>
@@ -17434,8 +17433,8 @@
       <c r="A107" s="48" t="s">
         <v>664</v>
       </c>
-      <c r="B107" s="48" t="s">
-        <v>3</v>
+      <c r="B107" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C107" s="48" t="s">
         <v>579</v>
@@ -17560,8 +17559,8 @@
       <c r="A108" s="49" t="s">
         <v>666</v>
       </c>
-      <c r="B108" s="48" t="s">
-        <v>3</v>
+      <c r="B108" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C108" s="49" t="s">
         <v>579</v>
@@ -17686,8 +17685,8 @@
       <c r="A109" s="48" t="s">
         <v>668</v>
       </c>
-      <c r="B109" s="48" t="s">
-        <v>3</v>
+      <c r="B109" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C109" s="48" t="s">
         <v>579</v>
@@ -17808,8 +17807,8 @@
       <c r="A110" s="49" t="s">
         <v>670</v>
       </c>
-      <c r="B110" s="48" t="s">
-        <v>3</v>
+      <c r="B110" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C110" s="49" t="s">
         <v>579</v>
@@ -17940,8 +17939,8 @@
       <c r="A111" s="49" t="s">
         <v>675</v>
       </c>
-      <c r="B111" s="48" t="s">
-        <v>3</v>
+      <c r="B111" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C111" s="49" t="s">
         <v>579</v>
@@ -18066,8 +18065,8 @@
       <c r="A112" s="48" t="s">
         <v>677</v>
       </c>
-      <c r="B112" s="48" t="s">
-        <v>3</v>
+      <c r="B112" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C112" s="48" t="s">
         <v>579</v>
@@ -18192,8 +18191,8 @@
       <c r="A113" s="48" t="s">
         <v>679</v>
       </c>
-      <c r="B113" s="48" t="s">
-        <v>3</v>
+      <c r="B113" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C113" s="48" t="s">
         <v>579</v>
@@ -18318,8 +18317,8 @@
       <c r="A114" s="48" t="s">
         <v>681</v>
       </c>
-      <c r="B114" s="48" t="s">
-        <v>3</v>
+      <c r="B114" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C114" s="48" t="s">
         <v>579</v>
@@ -18444,8 +18443,8 @@
       <c r="A115" s="48" t="s">
         <v>683</v>
       </c>
-      <c r="B115" s="48" t="s">
-        <v>3</v>
+      <c r="B115" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C115" s="48" t="s">
         <v>579</v>
@@ -18570,8 +18569,8 @@
       <c r="A116" s="48" t="s">
         <v>685</v>
       </c>
-      <c r="B116" s="48" t="s">
-        <v>3</v>
+      <c r="B116" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C116" s="48" t="s">
         <v>579</v>
@@ -18696,8 +18695,8 @@
       <c r="A117" s="48" t="s">
         <v>687</v>
       </c>
-      <c r="B117" s="48" t="s">
-        <v>3</v>
+      <c r="B117" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C117" s="48" t="s">
         <v>579</v>
@@ -18822,8 +18821,8 @@
       <c r="A118" s="48" t="s">
         <v>689</v>
       </c>
-      <c r="B118" s="48" t="s">
-        <v>3</v>
+      <c r="B118" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C118" s="48" t="s">
         <v>579</v>
@@ -18948,8 +18947,8 @@
       <c r="A119" s="48" t="s">
         <v>691</v>
       </c>
-      <c r="B119" s="48" t="s">
-        <v>3</v>
+      <c r="B119" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C119" s="48" t="s">
         <v>579</v>
@@ -19074,8 +19073,8 @@
       <c r="A120" s="48" t="s">
         <v>693</v>
       </c>
-      <c r="B120" s="48" t="s">
-        <v>3</v>
+      <c r="B120" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C120" s="48" t="s">
         <v>579</v>
@@ -19200,8 +19199,8 @@
       <c r="A121" s="48" t="s">
         <v>695</v>
       </c>
-      <c r="B121" s="48" t="s">
-        <v>3</v>
+      <c r="B121" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C121" s="48" t="s">
         <v>579</v>
@@ -19326,8 +19325,8 @@
       <c r="A122" s="48" t="s">
         <v>697</v>
       </c>
-      <c r="B122" s="48" t="s">
-        <v>3</v>
+      <c r="B122" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C122" s="48" t="s">
         <v>579</v>
@@ -19452,8 +19451,8 @@
       <c r="A123" s="48" t="s">
         <v>699</v>
       </c>
-      <c r="B123" s="48" t="s">
-        <v>3</v>
+      <c r="B123" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C123" s="48" t="s">
         <v>579</v>
@@ -19578,8 +19577,8 @@
       <c r="A124" s="48" t="s">
         <v>701</v>
       </c>
-      <c r="B124" s="48" t="s">
-        <v>3</v>
+      <c r="B124" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C124" s="48" t="s">
         <v>579</v>
@@ -19704,8 +19703,8 @@
       <c r="A125" s="48" t="s">
         <v>703</v>
       </c>
-      <c r="B125" s="48" t="s">
-        <v>3</v>
+      <c r="B125" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C125" s="48" t="s">
         <v>579</v>
@@ -19830,8 +19829,8 @@
       <c r="A126" s="48" t="s">
         <v>705</v>
       </c>
-      <c r="B126" s="48" t="s">
-        <v>3</v>
+      <c r="B126" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C126" s="48" t="s">
         <v>579</v>
@@ -19956,8 +19955,8 @@
       <c r="A127" s="48" t="s">
         <v>707</v>
       </c>
-      <c r="B127" s="48" t="s">
-        <v>3</v>
+      <c r="B127" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C127" s="48" t="s">
         <v>579</v>
@@ -20082,8 +20081,8 @@
       <c r="A128" s="48" t="s">
         <v>709</v>
       </c>
-      <c r="B128" s="48" t="s">
-        <v>3</v>
+      <c r="B128" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C128" s="48" t="s">
         <v>579</v>
@@ -20208,8 +20207,8 @@
       <c r="A129" s="48" t="s">
         <v>711</v>
       </c>
-      <c r="B129" s="48" t="s">
-        <v>3</v>
+      <c r="B129" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C129" s="48" t="s">
         <v>579</v>
@@ -20334,8 +20333,8 @@
       <c r="A130" s="48" t="s">
         <v>713</v>
       </c>
-      <c r="B130" s="48" t="s">
-        <v>3</v>
+      <c r="B130" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C130" s="48" t="s">
         <v>579</v>
@@ -20460,8 +20459,8 @@
       <c r="A131" s="48" t="s">
         <v>715</v>
       </c>
-      <c r="B131" s="48" t="s">
-        <v>3</v>
+      <c r="B131" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C131" s="48" t="s">
         <v>579</v>
@@ -20586,8 +20585,8 @@
       <c r="A132" s="48" t="s">
         <v>717</v>
       </c>
-      <c r="B132" s="48" t="s">
-        <v>3</v>
+      <c r="B132" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C132" s="48" t="s">
         <v>579</v>
@@ -20712,8 +20711,8 @@
       <c r="A133" s="48" t="s">
         <v>719</v>
       </c>
-      <c r="B133" s="48" t="s">
-        <v>3</v>
+      <c r="B133" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C133" s="48" t="s">
         <v>579</v>
@@ -20838,8 +20837,8 @@
       <c r="A134" s="48" t="s">
         <v>721</v>
       </c>
-      <c r="B134" s="48" t="s">
-        <v>3</v>
+      <c r="B134" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C134" s="48" t="s">
         <v>579</v>
@@ -20964,8 +20963,8 @@
       <c r="A135" s="48" t="s">
         <v>723</v>
       </c>
-      <c r="B135" s="48" t="s">
-        <v>3</v>
+      <c r="B135" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C135" s="48" t="s">
         <v>579</v>
@@ -21090,8 +21089,8 @@
       <c r="A136" s="48" t="s">
         <v>725</v>
       </c>
-      <c r="B136" s="48" t="s">
-        <v>3</v>
+      <c r="B136" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C136" s="48" t="s">
         <v>579</v>
@@ -21216,8 +21215,8 @@
       <c r="A137" s="48" t="s">
         <v>727</v>
       </c>
-      <c r="B137" s="48" t="s">
-        <v>3</v>
+      <c r="B137" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C137" s="48" t="s">
         <v>579</v>
@@ -21342,8 +21341,8 @@
       <c r="A138" s="48" t="s">
         <v>729</v>
       </c>
-      <c r="B138" s="48" t="s">
-        <v>3</v>
+      <c r="B138" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C138" s="48" t="s">
         <v>579</v>
@@ -21468,8 +21467,8 @@
       <c r="A139" s="48" t="s">
         <v>731</v>
       </c>
-      <c r="B139" s="48" t="s">
-        <v>3</v>
+      <c r="B139" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C139" s="48" t="s">
         <v>579</v>
@@ -21594,8 +21593,8 @@
       <c r="A140" s="48" t="s">
         <v>733</v>
       </c>
-      <c r="B140" s="48" t="s">
-        <v>3</v>
+      <c r="B140" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C140" s="48" t="s">
         <v>579</v>
@@ -21720,8 +21719,8 @@
       <c r="A141" s="48" t="s">
         <v>735</v>
       </c>
-      <c r="B141" s="48" t="s">
-        <v>3</v>
+      <c r="B141" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C141" s="48" t="s">
         <v>579</v>
@@ -21846,8 +21845,8 @@
       <c r="A142" s="48" t="s">
         <v>737</v>
       </c>
-      <c r="B142" s="48" t="s">
-        <v>3</v>
+      <c r="B142" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C142" s="48" t="s">
         <v>579</v>
@@ -21972,8 +21971,8 @@
       <c r="A143" s="48" t="s">
         <v>739</v>
       </c>
-      <c r="B143" s="48" t="s">
-        <v>3</v>
+      <c r="B143" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C143" s="48" t="s">
         <v>579</v>
@@ -22098,8 +22097,8 @@
       <c r="A144" s="48" t="s">
         <v>741</v>
       </c>
-      <c r="B144" s="48" t="s">
-        <v>3</v>
+      <c r="B144" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C144" s="48" t="s">
         <v>579</v>
@@ -22224,8 +22223,8 @@
       <c r="A145" s="48" t="s">
         <v>743</v>
       </c>
-      <c r="B145" s="48" t="s">
-        <v>3</v>
+      <c r="B145" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C145" s="48" t="s">
         <v>579</v>
@@ -22350,8 +22349,8 @@
       <c r="A146" s="49" t="s">
         <v>745</v>
       </c>
-      <c r="B146" s="48" t="s">
-        <v>3</v>
+      <c r="B146" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C146" s="49" t="s">
         <v>579</v>
@@ -22476,8 +22475,8 @@
       <c r="A147" s="48" t="s">
         <v>747</v>
       </c>
-      <c r="B147" s="48" t="s">
-        <v>3</v>
+      <c r="B147" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C147" s="48" t="s">
         <v>579</v>
@@ -22598,8 +22597,8 @@
       <c r="A148" s="48" t="s">
         <v>749</v>
       </c>
-      <c r="B148" s="48" t="s">
-        <v>3</v>
+      <c r="B148" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C148" s="48" t="s">
         <v>579</v>
@@ -22721,18 +22720,18 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="W11:W16" r:id="rId2" display="amulla@zarca.com,vgrandhi@zarca.com" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="W14" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="W10" r:id="rId4" display="ayadav@zarca.com" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="W11" r:id="rId5" display="ayadav@zarca.com" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="W12" r:id="rId6" display="ayadav@zarca.com" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="W13" r:id="rId7" display="ayadav@zarca.com" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="CU10" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="CU11" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="CU12" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="CU13" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="W110" r:id="rId12" xr:uid="{F334040F-B257-46E6-A3B0-EA9A32666BEF}"/>
+    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com"/>
+    <hyperlink ref="W11:W16" r:id="rId2" display="amulla@zarca.com,vgrandhi@zarca.com"/>
+    <hyperlink ref="W14" r:id="rId3"/>
+    <hyperlink ref="W10" r:id="rId4" display="ayadav@zarca.com"/>
+    <hyperlink ref="W11" r:id="rId5" display="ayadav@zarca.com"/>
+    <hyperlink ref="W12" r:id="rId6" display="ayadav@zarca.com"/>
+    <hyperlink ref="W13" r:id="rId7" display="ayadav@zarca.com"/>
+    <hyperlink ref="CU10" r:id="rId8"/>
+    <hyperlink ref="CU11" r:id="rId9"/>
+    <hyperlink ref="CU12" r:id="rId10"/>
+    <hyperlink ref="CU13" r:id="rId11"/>
+    <hyperlink ref="W110" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>

</xml_diff>

<commit_message>
Regression of Data Import & Data Export
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="785">
   <si>
     <t>Environment</t>
   </si>
@@ -2500,6 +2500,12 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>Data Import Completed</t>
+  </si>
+  <si>
+    <t>Data Export Completed</t>
   </si>
 </sst>
 </file>
@@ -3266,8 +3272,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CZ148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B148"/>
+    <sheetView tabSelected="1" topLeftCell="CC1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CS18" sqref="CS18:CV19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5946,10 +5952,18 @@
       <c r="CP18" s="19"/>
       <c r="CQ18" s="1"/>
       <c r="CR18" s="1"/>
-      <c r="CS18" s="1"/>
-      <c r="CT18" s="1"/>
-      <c r="CU18" s="1"/>
-      <c r="CV18" s="1"/>
+      <c r="CS18" s="25" t="s">
+        <v>557</v>
+      </c>
+      <c r="CT18" s="51" t="s">
+        <v>553</v>
+      </c>
+      <c r="CU18" s="23" t="s">
+        <v>558</v>
+      </c>
+      <c r="CV18" s="1" t="s">
+        <v>783</v>
+      </c>
       <c r="CW18" s="1"/>
       <c r="CX18" s="1"/>
       <c r="CY18" s="1"/>
@@ -6072,10 +6086,18 @@
       <c r="CP19" s="19"/>
       <c r="CQ19" s="1"/>
       <c r="CR19" s="1"/>
-      <c r="CS19" s="1"/>
-      <c r="CT19" s="1"/>
-      <c r="CU19" s="1"/>
-      <c r="CV19" s="1"/>
+      <c r="CS19" s="25" t="s">
+        <v>557</v>
+      </c>
+      <c r="CT19" s="51" t="s">
+        <v>553</v>
+      </c>
+      <c r="CU19" s="23" t="s">
+        <v>558</v>
+      </c>
+      <c r="CV19" s="1" t="s">
+        <v>784</v>
+      </c>
       <c r="CW19" s="1"/>
       <c r="CX19" s="1"/>
       <c r="CY19" s="1"/>

</xml_diff>

<commit_message>
Added rest of the code files for Regression of Data Import & Data Export
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -3272,8 +3272,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CZ148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CC1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="CS18" sqref="CS18:CV19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4736,7 +4736,7 @@
         <v>186</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>572</v>
@@ -5840,7 +5840,7 @@
         <v>226</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>572</v>
@@ -5974,7 +5974,7 @@
         <v>250</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>572</v>

</xml_diff>

<commit_message>
New login Test cases
</commit_message>
<xml_diff>
--- a/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
+++ b/Engage/Engage-Smoke/src/main/resources/excelfiles/Engage_Smoke.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3CB56C-BE52-4146-8ACD-9787DF5460D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1906" uniqueCount="793">
   <si>
     <t>Environment</t>
   </si>
@@ -2517,11 +2516,26 @@
   <si>
     <t>Failure Reason</t>
   </si>
+  <si>
+    <t>School Customer Experience &amp; Student Survey Platform | K12 Insight</t>
+  </si>
+  <si>
+    <t>url("https://www.k12insight.com/static/img/home/k12-login/logo-k-12.png")</t>
+  </si>
+  <si>
+    <t>url("https://www.k12insight.com/static/img/home/k12-login/lets-talk-knowledge-base.png")</t>
+  </si>
+  <si>
+    <t>From K12 Insight: Reset Password</t>
+  </si>
+  <si>
+    <t>From Let's Talk!: Reset Password</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13">
     <font>
       <sz val="11"/>
@@ -2548,6 +2562,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2585,6 +2600,7 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2602,6 +2618,7 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -2786,19 +2803,19 @@
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Hyperlink 2 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Hyperlink 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="4"/>
+    <cellStyle name="Hyperlink 2 2" xfId="11"/>
+    <cellStyle name="Hyperlink 3" xfId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Normal 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 4 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 5" xfId="6" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 5 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal 6" xfId="7" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="9"/>
+    <cellStyle name="Normal 3" xfId="5"/>
+    <cellStyle name="Normal 3 2" xfId="12"/>
+    <cellStyle name="Normal 4" xfId="3"/>
+    <cellStyle name="Normal 4 2" xfId="10"/>
+    <cellStyle name="Normal 5" xfId="6"/>
+    <cellStyle name="Normal 5 2" xfId="13"/>
+    <cellStyle name="Normal 6" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3075,7 +3092,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3113,14 +3130,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3162,7 +3179,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -3293,9 +3310,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -3303,12 +3320,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CZ148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="CL64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CW79" sqref="CW79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4263,7 +4280,7 @@
         <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>568</v>
@@ -13975,7 +13992,7 @@
         <v>573</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C79" s="34" t="s">
         <v>575</v>
@@ -13995,13 +14012,25 @@
         <v>187</v>
       </c>
       <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
-      <c r="M79" s="1"/>
-      <c r="N79" s="1"/>
-      <c r="O79" s="31"/>
+      <c r="K79" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="L79" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="M79" s="1">
+        <v>80</v>
+      </c>
+      <c r="N79" s="1">
+        <v>5</v>
+      </c>
+      <c r="O79" s="31" t="s">
+        <v>790</v>
+      </c>
       <c r="P79" s="31"/>
-      <c r="Q79" s="1"/>
+      <c r="Q79" s="1">
+        <v>60</v>
+      </c>
       <c r="R79" s="1"/>
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
@@ -14080,12 +14109,24 @@
       <c r="CO79" s="27"/>
       <c r="CP79" s="27"/>
       <c r="CQ79" s="1"/>
-      <c r="CR79" s="27"/>
-      <c r="CS79" s="25"/>
-      <c r="CT79" s="26"/>
-      <c r="CU79" s="23"/>
-      <c r="CV79" s="1"/>
-      <c r="CW79" s="1"/>
+      <c r="CR79" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="CS79" s="25" t="s">
+        <v>554</v>
+      </c>
+      <c r="CT79" s="26" t="s">
+        <v>550</v>
+      </c>
+      <c r="CU79" s="23" t="s">
+        <v>555</v>
+      </c>
+      <c r="CV79" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="CW79" s="1" t="s">
+        <v>791</v>
+      </c>
       <c r="CX79" s="1"/>
       <c r="CY79" s="1"/>
       <c r="CZ79" s="1"/>
@@ -22781,19 +22822,19 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="W11:W16" r:id="rId2" display="amulla@zarca.com,vgrandhi@zarca.com" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="W14" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="W10" r:id="rId4" display="ayadav@zarca.com" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="W11" r:id="rId5" display="ayadav@zarca.com" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="W12" r:id="rId6" display="ayadav@zarca.com" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="W13" r:id="rId7" display="ayadav@zarca.com" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="CU10" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="CU11" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="CU12" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="CU13" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="CT5" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
-    <hyperlink ref="W110" r:id="rId13" xr:uid="{A022143D-4BF0-4E26-9A51-63744989B9A7}"/>
+    <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com"/>
+    <hyperlink ref="W11:W16" r:id="rId2" display="amulla@zarca.com,vgrandhi@zarca.com"/>
+    <hyperlink ref="W14" r:id="rId3"/>
+    <hyperlink ref="W10" r:id="rId4" display="ayadav@zarca.com"/>
+    <hyperlink ref="W11" r:id="rId5" display="ayadav@zarca.com"/>
+    <hyperlink ref="W12" r:id="rId6" display="ayadav@zarca.com"/>
+    <hyperlink ref="W13" r:id="rId7" display="ayadav@zarca.com"/>
+    <hyperlink ref="CU10" r:id="rId8"/>
+    <hyperlink ref="CU11" r:id="rId9"/>
+    <hyperlink ref="CU12" r:id="rId10"/>
+    <hyperlink ref="CU13" r:id="rId11"/>
+    <hyperlink ref="CT5" r:id="rId12"/>
+    <hyperlink ref="W110" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId14"/>

</xml_diff>